<commit_message>
streamlined pmc population to behave more similarly to the other populate methods
</commit_message>
<xml_diff>
--- a/Covid_19_Dataset_and_References/References/4.xlsx
+++ b/Covid_19_Dataset_and_References/References/4.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Desktop\2023USRAResearch\CovidClef2023\covidClef2023\Covid_19_Dataset_and_References\References\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FAF730-05B5-400B-B00D-9CC30AA1C86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F13885-E89C-4DC0-A3A1-554E3E16F1AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="90" windowWidth="17220" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="74">
   <si>
     <t>Doi</t>
   </si>
@@ -31,16 +31,10 @@
     <t>10.1148/radiol.2020200823</t>
   </si>
   <si>
-    <t>10.1148/radiol.2020200642.</t>
-  </si>
-  <si>
     <t>10.1148/radiol.2020201237</t>
   </si>
   <si>
     <t>10.1007/s00330-020-06829-2</t>
-  </si>
-  <si>
-    <t>10.2214/AJR.20.22959.</t>
   </si>
   <si>
     <t>10.1148/ryct.2020200107</t>
@@ -217,33 +211,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Objectives
-id="Par1"&gt;Rapid and accurate diagnosis of coronavirus disease 2019 (COVID-19) is critical during the epidemic.
- We aim to identify differences in CT imaging and clinical manifestations between pneumonia patients with and without COVID-19, and to develop and validate a diagnostic model for COVID-19 based on radiological semantic and clinical features alone.
-Methods
-id="Par2"&gt;A consecutive cohort of 70 COVID-19 and 66 non-COVID-19 pneumonia patients were retrospectively recruited from five institutions.
- Patients were divided into primary (n = 98) and validation (n = 38) cohorts.
- The chi-square test, Student’s t test, and Kruskal-Wallis H test were performed, comparing 1745 lesions and 67 features in the two groups.
- Three models were constructed using radiological semantic and clinical features through multivariate logistic regression.
- Diagnostic efficacies of developed models were quantified by receiver operating characteristic curve.
- Clinical usage was evaluated by decision curve analysis and nomogram.
-Results
-id="Par3"&gt;Eighteen radiological semantic features and seventeen clinical features were identified to be significantly different.
- Besides ground-glass opacities (p = 0.032) and consolidation (p = 0.001) in the lung periphery, the lesion size (1–3 cm) is also significant for the diagnosis of COVID-19 (p = 0.027).
- Lung score presents no significant difference (p = 0.417).
- Three diagnostic models achieved an area under the curve value as high as 0.986 (95% CI 0.966~1.000).
- The clinical and radiological semantic models provided a better diagnostic performance and more considerable net benefits.
-Conclusions
-id="Par4"&gt;Based on CT imaging and clinical manifestations alone, the pneumonia patients with and without COVID-19 can be distinguished.
- A model composed of radiological semantic and clinical features has an excellent performance for the diagnosis of COVID-19.
-Key Points
-id="Par5"&gt;
-            • Based on CT imaging and clinical manifestations alone, the pneumonia patients with and without COVID-19 can be distinguished.
-Electronic supplementary material
-The online version of this article (10.1007/s00330-020-06829-2) contains supplementary material, which is available to authorized users.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Purpose
 To study the extent of pulmonary involvement in coronavirus 19 (COVID-19) with quantitative CT and to assess the impact of disease burden on opacity visibility on chest radiographs.
 Materials and Methods
@@ -262,21 +229,6 @@
 Conclusion
 QCTmass varied among patients with COVID-19. Chest radiographs had high specificity for detecting lung opacities in COVID-19 but a low sensitivity.
  QCTmass and combined opacity volume were significant determinants of opacity visibility on radiographs.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purpose
-id="Par1"&gt;To evaluate the diagnostic performance of chest CT to differentiate coronavirus disease 2019 (COVID-19) pneumonia in non-high-epidemic area in Japan.
-Materials and methods
-id="Par2"&gt;This retrospective study included 21 patients clinically suspected COVID-19 pneumonia and underwent chest CT more than 3 days after the symptom onset: six patients confirmed COVID-19 pneumonia by real-time reverse-transcription polymerase chain reaction (RT-PCR) and 15 patients proved uninfected.
- Using a Likert scale and its receiver operating characteristic curve analysis, two radiologists (R1/R2) evaluated the diagnostic performance of the five CT criteria: (1) ground glass opacity (GGO)-predominant lesions, (2) GGO- and peripheral-predominant lesions, (3) bilateral GGO-predominant lesions; (4) bilateral GGO- and peripheral-predominant lesions, and (5) bilateral GGO- and peripheral-predominant lesions without nodules, airway abnormalities, pleural effusion, and mediastinal lymphadenopathy.
-Results
-id="Par3"&gt;All patients confirmed COVID-19 pneumonia had bilateral GGO- and peripheral-predominant lesions without airway abnormalities, mediastinal lymphadenopathy, and pleural effusion.
- The five CT criteria showed moderate to excellent diagnostic performance with area under the curves (AUCs) ranging 0.77–0.88 for R1 and 0.78–0.92 for R2. The criterion (e) showed the highest AUC.
-Conclusion
-id="Par4"&gt;Chest CT would play a supplemental role to differentiate COVID-19 pneumonia from other respiratory diseases presenting with similar symptoms in a clinical setting.
-Electronic supplementary material
-The online version of this article (10.1007/s11604-020-00958-w) contains supplementary material, which is available to authorized users.
 </t>
   </si>
   <si>
@@ -329,379 +281,28 @@
 </t>
   </si>
   <si>
-    <t>[Harrison X.%Bai%NULL%2,    Ben%Hsieh%NULL%1,    Zeng%Xiong%NULL%1,    Kasey%Halsey%NULL%1,    Ji Whae%Choi%NULL%1,    Thi My Linh%Tran%NULL%1,    Ian%Pan%NULL%1,    Lin-Bo%Shi%NULL%1,    Dong-Cui%Wang%NULL%1,    Ji%Mei%NULL%1,    Xiao-Long%Jiang%NULL%1,    Qiu-Hua%Zeng%NULL%1,    Thomas K.%Egglin%NULL%1,    Ping-Feng%Hu%NULL%1,    Saurabh%Agarwal%NULL%1,    Fangfang%Xie%NULL%1,    Sha%Li%NULL%1,    Terrance%Healey%NULL%1,    Michael K.%Atalay%NULL%1,    Wei-Hua%Liao%liaoweihua2017@163.com%1,   Harrison X.%Bai%NULL%1,   Ben%Hsieh%NULL%1,   Zeng%Xiong%NULL%1,   Kasey%Halsey%NULL%1,   Ji Whae%Choi%NULL%1,   Thi My Linh%Tran%NULL%1,   Ian%Pan%NULL%1,   Lin-Bo%Shi%NULL%1,   Dong-Cui%Wang%NULL%1,   Ji%Mei%NULL%1,   Xiao-Long%Jiang%NULL%1,   Qiu-Hua%Zeng%NULL%1,   Thomas K.%Egglin%NULL%1,   Ping-Feng%Hu%NULL%1,   Saurabh%Agarwal%NULL%1,   Fangfang%Xie%NULL%1,   Sha%Li%NULL%1,   Terrance%Healey%NULL%1,   Michael K.%Atalay%NULL%1,   Wei-Hua%Liao%liaoweihua2017@163.com%1]</t>
-  </si>
-  <si>
-    <t>[Damiano%Caruso%NULL%1,    Marta%Zerunian%NULL%1,    Michela%Polici%NULL%1,    Francesco%Pucciarelli%NULL%1,    Tiziano%Polidori%NULL%1,    Carlotta%Rucci%NULL%1,    Gisella%Guido%NULL%1,    Benedetta%Bracci%NULL%1,    Chiara%de Dominicis%NULL%1,    Andrea%Laghi%andrea.laghi@uniroma1.it%1,   Damiano%Caruso%NULL%1,   Marta%Zerunian%NULL%1,   Michela%Polici%NULL%1,   Francesco%Pucciarelli%NULL%1,   Tiziano%Polidori%NULL%1,   Carlotta%Rucci%NULL%1,   Gisella%Guido%NULL%1,   Benedetta%Bracci%NULL%1,   Chiara%de Dominicis%NULL%1,   Andrea%Laghi%andrea.laghi@uniroma1.it%1]</t>
-  </si>
-  <si>
-    <t>[Xiaofeng%Chen%NULL%2,    Yanyan%Tang%NULL%1,    Yongkang%Mo%NULL%1,    Shengkai%Li%NULL%1,    Daiying%Lin%NULL%1,    Zhijian%Yang%NULL%1,    Zhiqi%Yang%NULL%1,    Hongfu%Sun%NULL%1,    Jinming%Qiu%NULL%1,    Yuting%Liao%NULL%1,    Jianning%Xiao%NULL%1,    Xiangguang%Chen%NULL%1,    Xianheng%Wu%NULL%1,    Renhua%Wu%NULL%1,    Zhuozhi%Dai%zhuozhi@ualberta.ca%1,   Xiaofeng%Chen%NULL%1,   Yanyan%Tang%NULL%1,   Yongkang%Mo%NULL%1,   Shengkai%Li%NULL%1,   Daiying%Lin%NULL%1,   Zhijian%Yang%NULL%1,   Zhiqi%Yang%NULL%1,   Hongfu%Sun%NULL%1,   Jinming%Qiu%NULL%1,   Yuting%Liao%NULL%1,   Jianning%Xiao%NULL%1,   Xiangguang%Chen%NULL%1,   Xianheng%Wu%NULL%1,   Renhua%Wu%NULL%1,   Zhuozhi%Dai%zhuozhi@ualberta.ca%1]</t>
-  </si>
-  <si>
-    <t>[Hyewon%Choi%NULL%2,    Xiaolong%Qi%NULL%1,    Soon Ho%Yoon%yshoka@gmail.com%1,    Sang Joon%Park%NULL%1,    Kyung Hee%Lee%NULL%1,    Jin Yong%Kim%NULL%1,    Young Kyung%Lee%NULL%1,    Hongseok%Ko%NULL%1,    Ki Hwan%Kim%NULL%1,    Chang Min%Park%NULL%1,    Yun-Hyeon%Kim%NULL%1,    Junqiang%Lei%NULL%1,    Jung Hee%Hong%NULL%1,    Hyungjin%Kim%NULL%1,    Eui Jin%Hwang%NULL%1,    Seung Jin%Yoo%NULL%1,    Ju Gang%Nam%NULL%1,    Chang Hyun%Lee%NULL%1,    Jin Mo%Goo%NULL%1,   Hyewon%Choi%NULL%1,   Xiaolong%Qi%NULL%1,   Soon Ho%Yoon%yshoka@gmail.com%1,   Sang Joon%Park%NULL%1,   Kyung Hee%Lee%NULL%1,   Jin Yong%Kim%NULL%1,   Young Kyung%Lee%NULL%1,   Hongseok%Ko%NULL%1,   Ki Hwan%Kim%NULL%1,   Chang Min%Park%NULL%1,   Yun-Hyeon%Kim%NULL%1,   Junqiang%Lei%NULL%1,   Jung Hee%Hong%NULL%1,   Hyungjin%Kim%NULL%1,   Eui Jin%Hwang%NULL%1,   Seung Jin%Yoo%NULL%1,   Ju Gang%Nam%NULL%1,   Chang Hyun%Lee%NULL%1,   Jin Mo%Goo%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Yuki%Himoto%yukihimoto@gmail.com%2,    Akihiko%Sakata%NULL%1,    Mitsuhiro%Kirita%NULL%1,    Takashi%Hiroi%NULL%1,    Ken-ichiro%Kobayashi%NULL%1,    Kenji%Kubo%NULL%1,    Hyunjin%Kim%NULL%1,    Azusa%Nishimoto%NULL%1,    Chikara%Maeda%NULL%1,    Akira%Kawamura%NULL%1,    Nobuhiro%Komiya%NULL%1,    Shigeaki%Umeoka%NULL%1,   Yuki%Himoto%yukihimoto@gmail.com%1,   Akihiko%Sakata%NULL%1,   Mitsuhiro%Kirita%NULL%1,   Takashi%Hiroi%NULL%1,   Ken-ichiro%Kobayashi%NULL%1,   Kenji%Kubo%NULL%1,   Hyunjin%Kim%NULL%1,   Azusa%Nishimoto%NULL%1,   Chikara%Maeda%NULL%1,   Akira%Kawamura%NULL%1,   Nobuhiro%Komiya%NULL%1,   Shigeaki%Umeoka%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Chunqin%Long%NULL%2,    Huaxiang%Xu%NULL%1,    Qinglin%Shen%NULL%1,    Xianghai%Zhang%NULL%1,    Bing%Fan%26171381@qq.com%1,    Chuanhong%Wang%NULL%1,    Bingliang%Zeng%NULL%1,    Zicong%Li%NULL%1,    Xiaofen%Li%NULL%1,    Honglu%Li%NULL%1,   Chunqin%Long%NULL%1,   Huaxiang%Xu%NULL%1,   Qinglin%Shen%NULL%1,   Xianghai%Zhang%NULL%1,   Bing%Fan%26171381@qq.com%1,   Chuanhong%Wang%NULL%1,   Bingliang%Zeng%NULL%1,   Zicong%Li%NULL%1,   Xiaofen%Li%NULL%1,   Honglu%Li%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,   Christopher%Gieraerts%NULL%0,   Yves%De Bruecker%NULL%0,   Lode%Janssen%NULL%0,   Hanne%Valgaeren%NULL%0,   Dagmar%Obbels%NULL%0,   Marc%Gillis%NULL%0,   Marc%Van Ranst%NULL%0,   Johan%Frans%NULL%0,   Annick%Demeyere%NULL%0,   Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
-    <t>[Wanbo%Zhu%NULL%0, Kai%Xie%NULL%2, Kai%Xie%NULL%0, Hui%Lu%NULL%1, Lei%Xu%bayinhexl@126.com%1, Shusheng%Zhou%zhouss108@163.com%1, Shiyuan%Fang%fangshiyuan2008@126.com%1]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0, Christopher%Gieraerts%NULL%2, Christopher%Gieraerts%NULL%0, Yves%De Bruecker%NULL%2, Yves%De Bruecker%NULL%0, Lode%Janssen%NULL%2, Lode%Janssen%NULL%0, Hanne%Valgaeren%NULL%2, Hanne%Valgaeren%NULL%0, Dagmar%Obbels%NULL%2, Dagmar%Obbels%NULL%0, Marc%Gillis%NULL%2, Marc%Gillis%NULL%0, Marc%Van Ranst%NULL%2, Marc%Van Ranst%NULL%0, Johan%Frans%NULL%1, Annick%Demeyere%NULL%2, Annick%Demeyere%NULL%0, Rolf%Symons%rolf.symons@imelda.be%2, Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
     <t>10.1016/j.ajem.2020.04.051</t>
   </si>
   <si>
-    <t>[Harrison X.%Bai%NULL%2,     Ben%Hsieh%NULL%1,     Zeng%Xiong%NULL%1,     Kasey%Halsey%NULL%1,     Ji Whae%Choi%NULL%1,     Thi My Linh%Tran%NULL%1,     Ian%Pan%NULL%1,     Lin-Bo%Shi%NULL%1,     Dong-Cui%Wang%NULL%1,     Ji%Mei%NULL%1,     Xiao-Long%Jiang%NULL%1,     Qiu-Hua%Zeng%NULL%1,     Thomas K.%Egglin%NULL%1,     Ping-Feng%Hu%NULL%1,     Saurabh%Agarwal%NULL%1,     Fangfang%Xie%NULL%1,     Sha%Li%NULL%1,     Terrance%Healey%NULL%1,     Michael K.%Atalay%NULL%1,     Wei-Hua%Liao%liaoweihua2017@163.com%1,    Harrison X.%Bai%NULL%1,    Ben%Hsieh%NULL%1,    Zeng%Xiong%NULL%1,    Kasey%Halsey%NULL%1,    Ji Whae%Choi%NULL%1,    Thi My Linh%Tran%NULL%1,    Ian%Pan%NULL%1,    Lin-Bo%Shi%NULL%1,    Dong-Cui%Wang%NULL%1,    Ji%Mei%NULL%1,    Xiao-Long%Jiang%NULL%1,    Qiu-Hua%Zeng%NULL%1,    Thomas K.%Egglin%NULL%1,    Ping-Feng%Hu%NULL%1,    Saurabh%Agarwal%NULL%1,    Fangfang%Xie%NULL%1,    Sha%Li%NULL%1,    Terrance%Healey%NULL%1,    Michael K.%Atalay%NULL%1,    Wei-Hua%Liao%liaoweihua2017@163.com%1]</t>
-  </si>
-  <si>
-    <t>[Damiano%Caruso%NULL%1,     Marta%Zerunian%NULL%1,     Michela%Polici%NULL%1,     Francesco%Pucciarelli%NULL%1,     Tiziano%Polidori%NULL%1,     Carlotta%Rucci%NULL%1,     Gisella%Guido%NULL%1,     Benedetta%Bracci%NULL%1,     Chiara%de Dominicis%NULL%1,     Andrea%Laghi%andrea.laghi@uniroma1.it%1,    Damiano%Caruso%NULL%1,    Marta%Zerunian%NULL%1,    Michela%Polici%NULL%1,    Francesco%Pucciarelli%NULL%1,    Tiziano%Polidori%NULL%1,    Carlotta%Rucci%NULL%1,    Gisella%Guido%NULL%1,    Benedetta%Bracci%NULL%1,    Chiara%de Dominicis%NULL%1,    Andrea%Laghi%andrea.laghi@uniroma1.it%1]</t>
-  </si>
-  <si>
-    <t>[Xiaofeng%Chen%NULL%2,     Yanyan%Tang%NULL%1,     Yongkang%Mo%NULL%1,     Shengkai%Li%NULL%1,     Daiying%Lin%NULL%1,     Zhijian%Yang%NULL%1,     Zhiqi%Yang%NULL%1,     Hongfu%Sun%NULL%1,     Jinming%Qiu%NULL%1,     Yuting%Liao%NULL%1,     Jianning%Xiao%NULL%1,     Xiangguang%Chen%NULL%1,     Xianheng%Wu%NULL%1,     Renhua%Wu%NULL%1,     Zhuozhi%Dai%zhuozhi@ualberta.ca%1,    Xiaofeng%Chen%NULL%1,    Yanyan%Tang%NULL%1,    Yongkang%Mo%NULL%1,    Shengkai%Li%NULL%1,    Daiying%Lin%NULL%1,    Zhijian%Yang%NULL%1,    Zhiqi%Yang%NULL%1,    Hongfu%Sun%NULL%1,    Jinming%Qiu%NULL%1,    Yuting%Liao%NULL%1,    Jianning%Xiao%NULL%1,    Xiangguang%Chen%NULL%1,    Xianheng%Wu%NULL%1,    Renhua%Wu%NULL%1,    Zhuozhi%Dai%zhuozhi@ualberta.ca%1]</t>
-  </si>
-  <si>
-    <t>[Hyewon%Choi%NULL%2,     Xiaolong%Qi%NULL%1,     Soon Ho%Yoon%yshoka@gmail.com%1,     Sang Joon%Park%NULL%1,     Kyung Hee%Lee%NULL%1,     Jin Yong%Kim%NULL%1,     Young Kyung%Lee%NULL%1,     Hongseok%Ko%NULL%1,     Ki Hwan%Kim%NULL%1,     Chang Min%Park%NULL%1,     Yun-Hyeon%Kim%NULL%1,     Junqiang%Lei%NULL%1,     Jung Hee%Hong%NULL%1,     Hyungjin%Kim%NULL%1,     Eui Jin%Hwang%NULL%1,     Seung Jin%Yoo%NULL%1,     Ju Gang%Nam%NULL%1,     Chang Hyun%Lee%NULL%1,     Jin Mo%Goo%NULL%1,    Hyewon%Choi%NULL%1,    Xiaolong%Qi%NULL%1,    Soon Ho%Yoon%yshoka@gmail.com%1,    Sang Joon%Park%NULL%1,    Kyung Hee%Lee%NULL%1,    Jin Yong%Kim%NULL%1,    Young Kyung%Lee%NULL%1,    Hongseok%Ko%NULL%1,    Ki Hwan%Kim%NULL%1,    Chang Min%Park%NULL%1,    Yun-Hyeon%Kim%NULL%1,    Junqiang%Lei%NULL%1,    Jung Hee%Hong%NULL%1,    Hyungjin%Kim%NULL%1,    Eui Jin%Hwang%NULL%1,    Seung Jin%Yoo%NULL%1,    Ju Gang%Nam%NULL%1,    Chang Hyun%Lee%NULL%1,    Jin Mo%Goo%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Yuki%Himoto%yukihimoto@gmail.com%2,     Akihiko%Sakata%NULL%1,     Mitsuhiro%Kirita%NULL%1,     Takashi%Hiroi%NULL%1,     Ken-ichiro%Kobayashi%NULL%1,     Kenji%Kubo%NULL%1,     Hyunjin%Kim%NULL%1,     Azusa%Nishimoto%NULL%1,     Chikara%Maeda%NULL%1,     Akira%Kawamura%NULL%1,     Nobuhiro%Komiya%NULL%1,     Shigeaki%Umeoka%NULL%1,    Yuki%Himoto%yukihimoto@gmail.com%1,    Akihiko%Sakata%NULL%1,    Mitsuhiro%Kirita%NULL%1,    Takashi%Hiroi%NULL%1,    Ken-ichiro%Kobayashi%NULL%1,    Kenji%Kubo%NULL%1,    Hyunjin%Kim%NULL%1,    Azusa%Nishimoto%NULL%1,    Chikara%Maeda%NULL%1,    Akira%Kawamura%NULL%1,    Nobuhiro%Komiya%NULL%1,    Shigeaki%Umeoka%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Chunqin%Long%NULL%2,     Huaxiang%Xu%NULL%1,     Qinglin%Shen%NULL%1,     Xianghai%Zhang%NULL%1,     Bing%Fan%26171381@qq.com%1,     Chuanhong%Wang%NULL%1,     Bingliang%Zeng%NULL%1,     Zicong%Li%NULL%1,     Xiaofen%Li%NULL%1,     Honglu%Li%NULL%1,    Chunqin%Long%NULL%1,    Huaxiang%Xu%NULL%1,    Qinglin%Shen%NULL%1,    Xianghai%Zhang%NULL%1,    Bing%Fan%26171381@qq.com%1,    Chuanhong%Wang%NULL%1,    Bingliang%Zeng%NULL%1,    Zicong%Li%NULL%1,    Xiaofen%Li%NULL%1,    Honglu%Li%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%3,    Christopher%Gieraerts%NULL%1,    Yves%De Bruecker%NULL%1,    Lode%Janssen%NULL%1,    Hanne%Valgaeren%NULL%1,    Dagmar%Obbels%NULL%1,    Marc%Gillis%NULL%1,    Marc%Van Ranst%NULL%0,    Johan%Frans%NULL%1,    Annick%Demeyere%NULL%1,    Rolf%Symons%rolf.symons@imelda.be%1]</t>
-  </si>
-  <si>
-    <t>[Wanbo%Zhu%NULL%0,  Kai%Xie%NULL%5,  Kai%Xie%NULL%0,  Hui%Lu%NULL%3,  Lei%Xu%bayinhexl@126.com%4,  Shusheng%Zhou%zhouss108@163.com%3,  Shiyuan%Fang%fangshiyuan2008@126.com%3]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,  Christopher%Gieraerts%NULL%4,  Christopher%Gieraerts%NULL%0,  Yves%De Bruecker%NULL%4,  Yves%De Bruecker%NULL%0,  Lode%Janssen%NULL%4,  Lode%Janssen%NULL%0,  Hanne%Valgaeren%NULL%4,  Hanne%Valgaeren%NULL%0,  Dagmar%Obbels%NULL%4,  Dagmar%Obbels%NULL%0,  Marc%Gillis%NULL%4,  Marc%Gillis%NULL%0,  Marc%Van Ranst%NULL%4,  Marc%Van Ranst%NULL%0,  Johan%Frans%NULL%3,  Annick%Demeyere%NULL%4,  Annick%Demeyere%NULL%0,  Rolf%Symons%rolf.symons@imelda.be%5,  Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
-    <t>[Harrison X.%Bai%NULL%2,      Ben%Hsieh%NULL%1,      Zeng%Xiong%NULL%1,      Kasey%Halsey%NULL%1,      Ji Whae%Choi%NULL%1,      Thi My Linh%Tran%NULL%1,      Ian%Pan%NULL%1,      Lin-Bo%Shi%NULL%1,      Dong-Cui%Wang%NULL%1,      Ji%Mei%NULL%1,      Xiao-Long%Jiang%NULL%1,      Qiu-Hua%Zeng%NULL%1,      Thomas K.%Egglin%NULL%1,      Ping-Feng%Hu%NULL%1,      Saurabh%Agarwal%NULL%1,      Fangfang%Xie%NULL%1,      Sha%Li%NULL%1,      Terrance%Healey%NULL%1,      Michael K.%Atalay%NULL%1,      Wei-Hua%Liao%liaoweihua2017@163.com%1,     Harrison X.%Bai%NULL%1,     Ben%Hsieh%NULL%1,     Zeng%Xiong%NULL%1,     Kasey%Halsey%NULL%1,     Ji Whae%Choi%NULL%1,     Thi My Linh%Tran%NULL%1,     Ian%Pan%NULL%1,     Lin-Bo%Shi%NULL%1,     Dong-Cui%Wang%NULL%1,     Ji%Mei%NULL%1,     Xiao-Long%Jiang%NULL%1,     Qiu-Hua%Zeng%NULL%1,     Thomas K.%Egglin%NULL%1,     Ping-Feng%Hu%NULL%1,     Saurabh%Agarwal%NULL%1,     Fangfang%Xie%NULL%1,     Sha%Li%NULL%1,     Terrance%Healey%NULL%1,     Michael K.%Atalay%NULL%1,     Wei-Hua%Liao%liaoweihua2017@163.com%1]</t>
-  </si>
-  <si>
-    <t>[Damiano%Caruso%NULL%1,      Marta%Zerunian%NULL%1,      Michela%Polici%NULL%1,      Francesco%Pucciarelli%NULL%1,      Tiziano%Polidori%NULL%1,      Carlotta%Rucci%NULL%1,      Gisella%Guido%NULL%1,      Benedetta%Bracci%NULL%1,      Chiara%de Dominicis%NULL%1,      Andrea%Laghi%andrea.laghi@uniroma1.it%1,     Damiano%Caruso%NULL%1,     Marta%Zerunian%NULL%1,     Michela%Polici%NULL%1,     Francesco%Pucciarelli%NULL%1,     Tiziano%Polidori%NULL%1,     Carlotta%Rucci%NULL%1,     Gisella%Guido%NULL%1,     Benedetta%Bracci%NULL%1,     Chiara%de Dominicis%NULL%1,     Andrea%Laghi%andrea.laghi@uniroma1.it%1]</t>
-  </si>
-  <si>
-    <t>[Xiaofeng%Chen%NULL%2,      Yanyan%Tang%NULL%1,      Yongkang%Mo%NULL%1,      Shengkai%Li%NULL%1,      Daiying%Lin%NULL%1,      Zhijian%Yang%NULL%1,      Zhiqi%Yang%NULL%1,      Hongfu%Sun%NULL%1,      Jinming%Qiu%NULL%1,      Yuting%Liao%NULL%1,      Jianning%Xiao%NULL%1,      Xiangguang%Chen%NULL%1,      Xianheng%Wu%NULL%1,      Renhua%Wu%NULL%1,      Zhuozhi%Dai%zhuozhi@ualberta.ca%1,     Xiaofeng%Chen%NULL%1,     Yanyan%Tang%NULL%1,     Yongkang%Mo%NULL%1,     Shengkai%Li%NULL%1,     Daiying%Lin%NULL%1,     Zhijian%Yang%NULL%1,     Zhiqi%Yang%NULL%1,     Hongfu%Sun%NULL%1,     Jinming%Qiu%NULL%1,     Yuting%Liao%NULL%1,     Jianning%Xiao%NULL%1,     Xiangguang%Chen%NULL%1,     Xianheng%Wu%NULL%1,     Renhua%Wu%NULL%1,     Zhuozhi%Dai%zhuozhi@ualberta.ca%1]</t>
-  </si>
-  <si>
-    <t>[Hyewon%Choi%NULL%2,      Xiaolong%Qi%NULL%1,      Soon Ho%Yoon%yshoka@gmail.com%1,      Sang Joon%Park%NULL%1,      Kyung Hee%Lee%NULL%1,      Jin Yong%Kim%NULL%1,      Young Kyung%Lee%NULL%1,      Hongseok%Ko%NULL%1,      Ki Hwan%Kim%NULL%1,      Chang Min%Park%NULL%1,      Yun-Hyeon%Kim%NULL%1,      Junqiang%Lei%NULL%1,      Jung Hee%Hong%NULL%1,      Hyungjin%Kim%NULL%1,      Eui Jin%Hwang%NULL%1,      Seung Jin%Yoo%NULL%1,      Ju Gang%Nam%NULL%1,      Chang Hyun%Lee%NULL%1,      Jin Mo%Goo%NULL%1,     Hyewon%Choi%NULL%1,     Xiaolong%Qi%NULL%1,     Soon Ho%Yoon%yshoka@gmail.com%1,     Sang Joon%Park%NULL%1,     Kyung Hee%Lee%NULL%1,     Jin Yong%Kim%NULL%1,     Young Kyung%Lee%NULL%1,     Hongseok%Ko%NULL%1,     Ki Hwan%Kim%NULL%1,     Chang Min%Park%NULL%1,     Yun-Hyeon%Kim%NULL%1,     Junqiang%Lei%NULL%1,     Jung Hee%Hong%NULL%1,     Hyungjin%Kim%NULL%1,     Eui Jin%Hwang%NULL%1,     Seung Jin%Yoo%NULL%1,     Ju Gang%Nam%NULL%1,     Chang Hyun%Lee%NULL%1,     Jin Mo%Goo%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Yuki%Himoto%yukihimoto@gmail.com%2,      Akihiko%Sakata%NULL%1,      Mitsuhiro%Kirita%NULL%1,      Takashi%Hiroi%NULL%1,      Ken-ichiro%Kobayashi%NULL%1,      Kenji%Kubo%NULL%1,      Hyunjin%Kim%NULL%1,      Azusa%Nishimoto%NULL%1,      Chikara%Maeda%NULL%1,      Akira%Kawamura%NULL%1,      Nobuhiro%Komiya%NULL%1,      Shigeaki%Umeoka%NULL%1,     Yuki%Himoto%yukihimoto@gmail.com%1,     Akihiko%Sakata%NULL%1,     Mitsuhiro%Kirita%NULL%1,     Takashi%Hiroi%NULL%1,     Ken-ichiro%Kobayashi%NULL%1,     Kenji%Kubo%NULL%1,     Hyunjin%Kim%NULL%1,     Azusa%Nishimoto%NULL%1,     Chikara%Maeda%NULL%1,     Akira%Kawamura%NULL%1,     Nobuhiro%Komiya%NULL%1,     Shigeaki%Umeoka%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Chunqin%Long%NULL%2,      Huaxiang%Xu%NULL%1,      Qinglin%Shen%NULL%1,      Xianghai%Zhang%NULL%1,      Bing%Fan%26171381@qq.com%1,      Chuanhong%Wang%NULL%1,      Bingliang%Zeng%NULL%1,      Zicong%Li%NULL%1,      Xiaofen%Li%NULL%1,      Honglu%Li%NULL%1,     Chunqin%Long%NULL%1,     Huaxiang%Xu%NULL%1,     Qinglin%Shen%NULL%1,     Xianghai%Zhang%NULL%1,     Bing%Fan%26171381@qq.com%1,     Chuanhong%Wang%NULL%1,     Bingliang%Zeng%NULL%1,     Zicong%Li%NULL%1,     Xiaofen%Li%NULL%1,     Honglu%Li%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%3,     Christopher%Gieraerts%NULL%1,     Yves%De Bruecker%NULL%1,     Lode%Janssen%NULL%1,     Hanne%Valgaeren%NULL%1,     Dagmar%Obbels%NULL%1,     Marc%Gillis%NULL%1,     Marc%Van Ranst%NULL%0,     Johan%Frans%NULL%1,     Annick%Demeyere%NULL%1,     Rolf%Symons%rolf.symons@imelda.be%1]</t>
-  </si>
-  <si>
-    <t>[Wanbo%Zhu%NULL%0,   Kai%Xie%NULL%2,   Kai%Xie%NULL%0,   Hui%Lu%NULL%1,   Lei%Xu%bayinhexl@126.com%1,   Shusheng%Zhou%zhouss108@163.com%1,   Shiyuan%Fang%fangshiyuan2008@126.com%1]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,   Christopher%Gieraerts%NULL%2,   Christopher%Gieraerts%NULL%0,   Yves%De Bruecker%NULL%2,   Yves%De Bruecker%NULL%0,   Lode%Janssen%NULL%2,   Lode%Janssen%NULL%0,   Hanne%Valgaeren%NULL%2,   Hanne%Valgaeren%NULL%0,   Dagmar%Obbels%NULL%2,   Dagmar%Obbels%NULL%0,   Marc%Gillis%NULL%2,   Marc%Gillis%NULL%0,   Marc%Van Ranst%NULL%2,   Marc%Van Ranst%NULL%0,   Johan%Frans%NULL%1,   Annick%Demeyere%NULL%2,   Annick%Demeyere%NULL%0,   Rolf%Symons%rolf.symons@imelda.be%2,   Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
     <t>Other found locations</t>
   </si>
   <si>
-    <t>[Harrison X.%Bai%NULL%2,       Ben%Hsieh%NULL%1,       Zeng%Xiong%NULL%1,       Kasey%Halsey%NULL%1,       Ji Whae%Choi%NULL%1,       Thi My Linh%Tran%NULL%1,       Ian%Pan%NULL%1,       Lin-Bo%Shi%NULL%1,       Dong-Cui%Wang%NULL%1,       Ji%Mei%NULL%1,       Xiao-Long%Jiang%NULL%1,       Qiu-Hua%Zeng%NULL%1,       Thomas K.%Egglin%NULL%1,       Ping-Feng%Hu%NULL%1,       Saurabh%Agarwal%NULL%1,       Fangfang%Xie%NULL%1,       Sha%Li%NULL%1,       Terrance%Healey%NULL%1,       Michael K.%Atalay%NULL%1,       Wei-Hua%Liao%liaoweihua2017@163.com%1,      Harrison X.%Bai%NULL%1,      Ben%Hsieh%NULL%1,      Zeng%Xiong%NULL%1,      Kasey%Halsey%NULL%1,      Ji Whae%Choi%NULL%1,      Thi My Linh%Tran%NULL%1,      Ian%Pan%NULL%1,      Lin-Bo%Shi%NULL%1,      Dong-Cui%Wang%NULL%1,      Ji%Mei%NULL%1,      Xiao-Long%Jiang%NULL%1,      Qiu-Hua%Zeng%NULL%1,      Thomas K.%Egglin%NULL%1,      Ping-Feng%Hu%NULL%1,      Saurabh%Agarwal%NULL%1,      Fangfang%Xie%NULL%1,      Sha%Li%NULL%1,      Terrance%Healey%NULL%1,      Michael K.%Atalay%NULL%1,      Wei-Hua%Liao%liaoweihua2017@163.com%1]</t>
-  </si>
-  <si>
     <t>_PMC</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>[Damiano%Caruso%NULL%2,       Marta%Zerunian%NULL%1,       Michela%Polici%NULL%1,       Francesco%Pucciarelli%NULL%1,       Tiziano%Polidori%NULL%1,       Carlotta%Rucci%NULL%1,       Gisella%Guido%NULL%1,       Benedetta%Bracci%NULL%1,       Chiara%de Dominicis%NULL%1,       Andrea%Laghi%andrea.laghi@uniroma1.it%1,      Damiano%Caruso%NULL%1,      Marta%Zerunian%NULL%1,      Michela%Polici%NULL%1,      Francesco%Pucciarelli%NULL%1,      Tiziano%Polidori%NULL%1,      Carlotta%Rucci%NULL%1,      Gisella%Guido%NULL%1,      Benedetta%Bracci%NULL%1,      Chiara%de Dominicis%NULL%1,      Andrea%Laghi%andrea.laghi@uniroma1.it%1]</t>
-  </si>
-  <si>
-    <t>[Xiaofeng%Chen%NULL%2,       Yanyan%Tang%NULL%1,       Yongkang%Mo%NULL%1,       Shengkai%Li%NULL%1,       Daiying%Lin%NULL%1,       Zhijian%Yang%NULL%1,       Zhiqi%Yang%NULL%1,       Hongfu%Sun%NULL%1,       Jinming%Qiu%NULL%1,       Yuting%Liao%NULL%1,       Jianning%Xiao%NULL%1,       Xiangguang%Chen%NULL%1,       Xianheng%Wu%NULL%1,       Renhua%Wu%NULL%1,       Zhuozhi%Dai%zhuozhi@ualberta.ca%1,      Xiaofeng%Chen%NULL%1,      Yanyan%Tang%NULL%1,      Yongkang%Mo%NULL%1,      Shengkai%Li%NULL%1,      Daiying%Lin%NULL%1,      Zhijian%Yang%NULL%1,      Zhiqi%Yang%NULL%1,      Hongfu%Sun%NULL%1,      Jinming%Qiu%NULL%1,      Yuting%Liao%NULL%1,      Jianning%Xiao%NULL%1,      Xiangguang%Chen%NULL%1,      Xianheng%Wu%NULL%1,      Renhua%Wu%NULL%1,      Zhuozhi%Dai%zhuozhi@ualberta.ca%1]</t>
-  </si>
-  <si>
     <t>_PMC_Springer</t>
   </si>
   <si>
-    <t>[Hyewon%Choi%NULL%2,       Xiaolong%Qi%NULL%1,       Soon Ho%Yoon%yshoka@gmail.com%1,       Sang Joon%Park%NULL%1,       Kyung Hee%Lee%NULL%1,       Jin Yong%Kim%NULL%1,       Young Kyung%Lee%NULL%1,       Hongseok%Ko%NULL%1,       Ki Hwan%Kim%NULL%1,       Chang Min%Park%NULL%1,       Yun-Hyeon%Kim%NULL%1,       Junqiang%Lei%NULL%1,       Jung Hee%Hong%NULL%1,       Hyungjin%Kim%NULL%1,       Eui Jin%Hwang%NULL%1,       Seung Jin%Yoo%NULL%1,       Ju Gang%Nam%NULL%1,       Chang Hyun%Lee%NULL%1,       Jin Mo%Goo%NULL%1,      Hyewon%Choi%NULL%1,      Xiaolong%Qi%NULL%1,      Soon Ho%Yoon%yshoka@gmail.com%1,      Sang Joon%Park%NULL%1,      Kyung Hee%Lee%NULL%1,      Jin Yong%Kim%NULL%1,      Young Kyung%Lee%NULL%1,      Hongseok%Ko%NULL%1,      Ki Hwan%Kim%NULL%1,      Chang Min%Park%NULL%1,      Yun-Hyeon%Kim%NULL%1,      Junqiang%Lei%NULL%1,      Jung Hee%Hong%NULL%1,      Hyungjin%Kim%NULL%1,      Eui Jin%Hwang%NULL%1,      Seung Jin%Yoo%NULL%1,      Ju Gang%Nam%NULL%1,      Chang Hyun%Lee%NULL%1,      Jin Mo%Goo%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Yuki%Himoto%yukihimoto@gmail.com%2,       Akihiko%Sakata%NULL%1,       Mitsuhiro%Kirita%NULL%1,       Takashi%Hiroi%NULL%1,       Ken-ichiro%Kobayashi%NULL%1,       Kenji%Kubo%NULL%1,       Hyunjin%Kim%NULL%1,       Azusa%Nishimoto%NULL%1,       Chikara%Maeda%NULL%1,       Akira%Kawamura%NULL%1,       Nobuhiro%Komiya%NULL%1,       Shigeaki%Umeoka%NULL%1,      Yuki%Himoto%yukihimoto@gmail.com%1,      Akihiko%Sakata%NULL%1,      Mitsuhiro%Kirita%NULL%1,      Takashi%Hiroi%NULL%1,      Ken-ichiro%Kobayashi%NULL%1,      Kenji%Kubo%NULL%1,      Hyunjin%Kim%NULL%1,      Azusa%Nishimoto%NULL%1,      Chikara%Maeda%NULL%1,      Akira%Kawamura%NULL%1,      Nobuhiro%Komiya%NULL%1,      Shigeaki%Umeoka%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Chunqin%Long%NULL%2,       Huaxiang%Xu%NULL%1,       Qinglin%Shen%NULL%1,       Xianghai%Zhang%NULL%1,       Bing%Fan%26171381@qq.com%1,       Chuanhong%Wang%NULL%1,       Bingliang%Zeng%NULL%1,       Zicong%Li%NULL%1,       Xiaofen%Li%NULL%1,       Honglu%Li%NULL%1,      Chunqin%Long%NULL%1,      Huaxiang%Xu%NULL%1,      Qinglin%Shen%NULL%1,      Xianghai%Zhang%NULL%1,      Bing%Fan%26171381@qq.com%1,      Chuanhong%Wang%NULL%1,      Bingliang%Zeng%NULL%1,      Zicong%Li%NULL%1,      Xiaofen%Li%NULL%1,      Honglu%Li%NULL%1]</t>
-  </si>
-  <si>
     <t>_PMC_elsevier</t>
   </si>
   <si>
-    <t>[Anthony%Dangis%NULL%4,      Christopher%Gieraerts%NULL%1,      Yves%De Bruecker%NULL%1,      Lode%Janssen%NULL%1,      Hanne%Valgaeren%NULL%1,      Dagmar%Obbels%NULL%1,      Marc%Gillis%NULL%1,      Marc%Van Ranst%NULL%0,      Johan%Frans%NULL%1,      Annick%Demeyere%NULL%1,      Rolf%Symons%rolf.symons@imelda.be%1]</t>
-  </si>
-  <si>
     <t>PMC7166306</t>
   </si>
   <si>
-    <t>[Wanbo%Zhu%NULL%0,    Kai%Xie%NULL%0,    Kai%Xie%NULL%0,    Hui%Lu%NULL%0,    Lei%Xu%bayinhexl@126.com%0,    Shusheng%Zhou%zhouss108@163.com%0,    Shiyuan%Fang%fangshiyuan2008@126.com%0]</t>
-  </si>
-  <si>
     <t>PMC7194021</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,    Christopher%Gieraerts%NULL%2,    Christopher%Gieraerts%NULL%0,    Yves%De Bruecker%NULL%2,    Yves%De Bruecker%NULL%0,    Lode%Janssen%NULL%2,    Lode%Janssen%NULL%0,    Hanne%Valgaeren%NULL%2,    Hanne%Valgaeren%NULL%0,    Dagmar%Obbels%NULL%2,    Dagmar%Obbels%NULL%0,    Marc%Gillis%NULL%2,    Marc%Gillis%NULL%0,    Marc%Van Ranst%NULL%0,    Marc%Van Ranst%NULL%0,    Johan%Frans%NULL%1,    Annick%Demeyere%NULL%2,    Annick%Demeyere%NULL%0,    Rolf%Symons%rolf.symons@imelda.be%2,    Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
-    <t>[Harrison X.%Bai%NULL%2,        Ben%Hsieh%NULL%1,        Zeng%Xiong%NULL%1,        Kasey%Halsey%NULL%1,        Ji Whae%Choi%NULL%1,        Thi My Linh%Tran%NULL%1,        Ian%Pan%NULL%1,        Lin-Bo%Shi%NULL%1,        Dong-Cui%Wang%NULL%1,        Ji%Mei%NULL%1,        Xiao-Long%Jiang%NULL%1,        Qiu-Hua%Zeng%NULL%1,        Thomas K.%Egglin%NULL%1,        Ping-Feng%Hu%NULL%1,        Saurabh%Agarwal%NULL%1,        Fangfang%Xie%NULL%1,        Sha%Li%NULL%1,        Terrance%Healey%NULL%1,        Michael K.%Atalay%NULL%1,        Wei-Hua%Liao%liaoweihua2017@163.com%1,       Harrison X.%Bai%NULL%1,       Ben%Hsieh%NULL%1,       Zeng%Xiong%NULL%1,       Kasey%Halsey%NULL%1,       Ji Whae%Choi%NULL%1,       Thi My Linh%Tran%NULL%1,       Ian%Pan%NULL%1,       Lin-Bo%Shi%NULL%1,       Dong-Cui%Wang%NULL%1,       Ji%Mei%NULL%1,       Xiao-Long%Jiang%NULL%1,       Qiu-Hua%Zeng%NULL%1,       Thomas K.%Egglin%NULL%1,       Ping-Feng%Hu%NULL%1,       Saurabh%Agarwal%NULL%1,       Fangfang%Xie%NULL%1,       Sha%Li%NULL%1,       Terrance%Healey%NULL%1,       Michael K.%Atalay%NULL%1,       Wei-Hua%Liao%liaoweihua2017@163.com%1]</t>
-  </si>
-  <si>
-    <t>[Damiano%Caruso%NULL%2,        Marta%Zerunian%NULL%1,        Michela%Polici%NULL%1,        Francesco%Pucciarelli%NULL%1,        Tiziano%Polidori%NULL%1,        Carlotta%Rucci%NULL%1,        Gisella%Guido%NULL%1,        Benedetta%Bracci%NULL%1,        Chiara%de Dominicis%NULL%1,        Andrea%Laghi%andrea.laghi@uniroma1.it%1,       Damiano%Caruso%NULL%1,       Marta%Zerunian%NULL%1,       Michela%Polici%NULL%1,       Francesco%Pucciarelli%NULL%1,       Tiziano%Polidori%NULL%1,       Carlotta%Rucci%NULL%1,       Gisella%Guido%NULL%1,       Benedetta%Bracci%NULL%1,       Chiara%de Dominicis%NULL%1,       Andrea%Laghi%andrea.laghi@uniroma1.it%1]</t>
-  </si>
-  <si>
-    <t>[Xiaofeng%Chen%NULL%2,        Yanyan%Tang%NULL%1,        Yongkang%Mo%NULL%1,        Shengkai%Li%NULL%1,        Daiying%Lin%NULL%1,        Zhijian%Yang%NULL%1,        Zhiqi%Yang%NULL%1,        Hongfu%Sun%NULL%1,        Jinming%Qiu%NULL%1,        Yuting%Liao%NULL%1,        Jianning%Xiao%NULL%1,        Xiangguang%Chen%NULL%1,        Xianheng%Wu%NULL%1,        Renhua%Wu%NULL%1,        Zhuozhi%Dai%zhuozhi@ualberta.ca%1,       Xiaofeng%Chen%NULL%1,       Yanyan%Tang%NULL%1,       Yongkang%Mo%NULL%1,       Shengkai%Li%NULL%1,       Daiying%Lin%NULL%1,       Zhijian%Yang%NULL%1,       Zhiqi%Yang%NULL%1,       Hongfu%Sun%NULL%1,       Jinming%Qiu%NULL%1,       Yuting%Liao%NULL%1,       Jianning%Xiao%NULL%1,       Xiangguang%Chen%NULL%1,       Xianheng%Wu%NULL%1,       Renhua%Wu%NULL%1,       Zhuozhi%Dai%zhuozhi@ualberta.ca%1]</t>
-  </si>
-  <si>
-    <t>[Hyewon%Choi%NULL%2,        Xiaolong%Qi%NULL%1,        Soon Ho%Yoon%yshoka@gmail.com%1,        Sang Joon%Park%NULL%1,        Kyung Hee%Lee%NULL%1,        Jin Yong%Kim%NULL%1,        Young Kyung%Lee%NULL%1,        Hongseok%Ko%NULL%1,        Ki Hwan%Kim%NULL%1,        Chang Min%Park%NULL%1,        Yun-Hyeon%Kim%NULL%1,        Junqiang%Lei%NULL%1,        Jung Hee%Hong%NULL%1,        Hyungjin%Kim%NULL%1,        Eui Jin%Hwang%NULL%1,        Seung Jin%Yoo%NULL%1,        Ju Gang%Nam%NULL%1,        Chang Hyun%Lee%NULL%1,        Jin Mo%Goo%NULL%1,       Hyewon%Choi%NULL%1,       Xiaolong%Qi%NULL%1,       Soon Ho%Yoon%yshoka@gmail.com%1,       Sang Joon%Park%NULL%1,       Kyung Hee%Lee%NULL%1,       Jin Yong%Kim%NULL%1,       Young Kyung%Lee%NULL%1,       Hongseok%Ko%NULL%1,       Ki Hwan%Kim%NULL%1,       Chang Min%Park%NULL%1,       Yun-Hyeon%Kim%NULL%1,       Junqiang%Lei%NULL%1,       Jung Hee%Hong%NULL%1,       Hyungjin%Kim%NULL%1,       Eui Jin%Hwang%NULL%1,       Seung Jin%Yoo%NULL%1,       Ju Gang%Nam%NULL%1,       Chang Hyun%Lee%NULL%1,       Jin Mo%Goo%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Yuki%Himoto%yukihimoto@gmail.com%2,        Akihiko%Sakata%NULL%1,        Mitsuhiro%Kirita%NULL%1,        Takashi%Hiroi%NULL%1,        Ken-ichiro%Kobayashi%NULL%1,        Kenji%Kubo%NULL%1,        Hyunjin%Kim%NULL%1,        Azusa%Nishimoto%NULL%1,        Chikara%Maeda%NULL%1,        Akira%Kawamura%NULL%1,        Nobuhiro%Komiya%NULL%1,        Shigeaki%Umeoka%NULL%1,       Yuki%Himoto%yukihimoto@gmail.com%1,       Akihiko%Sakata%NULL%1,       Mitsuhiro%Kirita%NULL%1,       Takashi%Hiroi%NULL%1,       Ken-ichiro%Kobayashi%NULL%1,       Kenji%Kubo%NULL%1,       Hyunjin%Kim%NULL%1,       Azusa%Nishimoto%NULL%1,       Chikara%Maeda%NULL%1,       Akira%Kawamura%NULL%1,       Nobuhiro%Komiya%NULL%1,       Shigeaki%Umeoka%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Chunqin%Long%NULL%2,        Huaxiang%Xu%NULL%1,        Qinglin%Shen%NULL%1,        Xianghai%Zhang%NULL%1,        Bing%Fan%26171381@qq.com%1,        Chuanhong%Wang%NULL%1,        Bingliang%Zeng%NULL%1,        Zicong%Li%NULL%1,        Xiaofen%Li%NULL%1,        Honglu%Li%NULL%1,       Chunqin%Long%NULL%1,       Huaxiang%Xu%NULL%1,       Qinglin%Shen%NULL%1,       Xianghai%Zhang%NULL%1,       Bing%Fan%26171381@qq.com%1,       Chuanhong%Wang%NULL%1,       Bingliang%Zeng%NULL%1,       Zicong%Li%NULL%1,       Xiaofen%Li%NULL%1,       Honglu%Li%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%4,       Christopher%Gieraerts%NULL%1,       Yves%De Bruecker%NULL%1,       Lode%Janssen%NULL%1,       Hanne%Valgaeren%NULL%1,       Dagmar%Obbels%NULL%1,       Marc%Gillis%NULL%1,       Marc%Van Ranst%NULL%0,       Johan%Frans%NULL%1,       Annick%Demeyere%NULL%1,       Rolf%Symons%rolf.symons@imelda.be%1]</t>
-  </si>
-  <si>
-    <t>[Wanbo%Zhu%NULL%0,     Kai%Xie%NULL%0,     Kai%Xie%NULL%0,     Hui%Lu%NULL%0,     Lei%Xu%bayinhexl@126.com%0,     Shusheng%Zhou%zhouss108@163.com%0,     Shiyuan%Fang%fangshiyuan2008@126.com%0]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,     Christopher%Gieraerts%NULL%2,     Christopher%Gieraerts%NULL%0,     Yves%De Bruecker%NULL%2,     Yves%De Bruecker%NULL%0,     Lode%Janssen%NULL%2,     Lode%Janssen%NULL%0,     Hanne%Valgaeren%NULL%2,     Hanne%Valgaeren%NULL%0,     Dagmar%Obbels%NULL%2,     Dagmar%Obbels%NULL%0,     Marc%Gillis%NULL%2,     Marc%Gillis%NULL%0,     Marc%Van Ranst%NULL%0,     Marc%Van Ranst%NULL%0,     Johan%Frans%NULL%1,     Annick%Demeyere%NULL%2,     Annick%Demeyere%NULL%0,     Rolf%Symons%rolf.symons@imelda.be%2,     Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,  Christopher%Gieraerts%NULL%2,  Christopher%Gieraerts%NULL%0,  Yves%De Bruecker%NULL%2,  Yves%De Bruecker%NULL%0,  Lode%Janssen%NULL%2,  Lode%Janssen%NULL%0,  Hanne%Valgaeren%NULL%2,  Hanne%Valgaeren%NULL%0,  Dagmar%Obbels%NULL%2,  Dagmar%Obbels%NULL%0,  Marc%Gillis%NULL%2,  Marc%Gillis%NULL%0,  Marc%Van Ranst%NULL%2,  Marc%Van Ranst%NULL%0,  Johan%Frans%NULL%1,  Annick%Demeyere%NULL%2,  Annick%Demeyere%NULL%0,  Rolf%Symons%rolf.symons@imelda.be%2,  Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
-    <t>[Harrison X.%Bai%NULL%2,         Ben%Hsieh%NULL%1,         Zeng%Xiong%NULL%1,         Kasey%Halsey%NULL%1,         Ji Whae%Choi%NULL%1,         Thi My Linh%Tran%NULL%1,         Ian%Pan%NULL%1,         Lin-Bo%Shi%NULL%1,         Dong-Cui%Wang%NULL%1,         Ji%Mei%NULL%1,         Xiao-Long%Jiang%NULL%1,         Qiu-Hua%Zeng%NULL%1,         Thomas K.%Egglin%NULL%1,         Ping-Feng%Hu%NULL%1,         Saurabh%Agarwal%NULL%1,         Fangfang%Xie%NULL%1,         Sha%Li%NULL%1,         Terrance%Healey%NULL%1,         Michael K.%Atalay%NULL%1,         Wei-Hua%Liao%liaoweihua2017@163.com%1,        Harrison X.%Bai%NULL%1,        Ben%Hsieh%NULL%1,        Zeng%Xiong%NULL%1,        Kasey%Halsey%NULL%1,        Ji Whae%Choi%NULL%1,        Thi My Linh%Tran%NULL%1,        Ian%Pan%NULL%1,        Lin-Bo%Shi%NULL%1,        Dong-Cui%Wang%NULL%1,        Ji%Mei%NULL%1,        Xiao-Long%Jiang%NULL%1,        Qiu-Hua%Zeng%NULL%1,        Thomas K.%Egglin%NULL%1,        Ping-Feng%Hu%NULL%1,        Saurabh%Agarwal%NULL%1,        Fangfang%Xie%NULL%1,        Sha%Li%NULL%1,        Terrance%Healey%NULL%1,        Michael K.%Atalay%NULL%1,        Wei-Hua%Liao%liaoweihua2017@163.com%1]</t>
-  </si>
-  <si>
-    <t>[Damiano%Caruso%NULL%2,         Marta%Zerunian%NULL%1,         Michela%Polici%NULL%1,         Francesco%Pucciarelli%NULL%1,         Tiziano%Polidori%NULL%1,         Carlotta%Rucci%NULL%1,         Gisella%Guido%NULL%1,         Benedetta%Bracci%NULL%1,         Chiara%de Dominicis%NULL%1,         Andrea%Laghi%andrea.laghi@uniroma1.it%1,        Damiano%Caruso%NULL%1,        Marta%Zerunian%NULL%1,        Michela%Polici%NULL%1,        Francesco%Pucciarelli%NULL%1,        Tiziano%Polidori%NULL%1,        Carlotta%Rucci%NULL%1,        Gisella%Guido%NULL%1,        Benedetta%Bracci%NULL%1,        Chiara%de Dominicis%NULL%1,        Andrea%Laghi%andrea.laghi@uniroma1.it%1]</t>
-  </si>
-  <si>
-    <t>[Xiaofeng%Chen%NULL%2,         Yanyan%Tang%NULL%1,         Yongkang%Mo%NULL%1,         Shengkai%Li%NULL%1,         Daiying%Lin%NULL%1,         Zhijian%Yang%NULL%1,         Zhiqi%Yang%NULL%1,         Hongfu%Sun%NULL%1,         Jinming%Qiu%NULL%1,         Yuting%Liao%NULL%1,         Jianning%Xiao%NULL%1,         Xiangguang%Chen%NULL%1,         Xianheng%Wu%NULL%1,         Renhua%Wu%NULL%1,         Zhuozhi%Dai%zhuozhi@ualberta.ca%1,        Xiaofeng%Chen%NULL%1,        Yanyan%Tang%NULL%1,        Yongkang%Mo%NULL%1,        Shengkai%Li%NULL%1,        Daiying%Lin%NULL%1,        Zhijian%Yang%NULL%1,        Zhiqi%Yang%NULL%1,        Hongfu%Sun%NULL%1,        Jinming%Qiu%NULL%1,        Yuting%Liao%NULL%1,        Jianning%Xiao%NULL%1,        Xiangguang%Chen%NULL%1,        Xianheng%Wu%NULL%1,        Renhua%Wu%NULL%1,        Zhuozhi%Dai%zhuozhi@ualberta.ca%1]</t>
-  </si>
-  <si>
-    <t>[Hyewon%Choi%NULL%2,         Xiaolong%Qi%NULL%1,         Soon Ho%Yoon%yshoka@gmail.com%1,         Sang Joon%Park%NULL%1,         Kyung Hee%Lee%NULL%1,         Jin Yong%Kim%NULL%1,         Young Kyung%Lee%NULL%1,         Hongseok%Ko%NULL%1,         Ki Hwan%Kim%NULL%1,         Chang Min%Park%NULL%1,         Yun-Hyeon%Kim%NULL%1,         Junqiang%Lei%NULL%1,         Jung Hee%Hong%NULL%1,         Hyungjin%Kim%NULL%1,         Eui Jin%Hwang%NULL%1,         Seung Jin%Yoo%NULL%1,         Ju Gang%Nam%NULL%1,         Chang Hyun%Lee%NULL%1,         Jin Mo%Goo%NULL%1,        Hyewon%Choi%NULL%1,        Xiaolong%Qi%NULL%1,        Soon Ho%Yoon%yshoka@gmail.com%1,        Sang Joon%Park%NULL%1,        Kyung Hee%Lee%NULL%1,        Jin Yong%Kim%NULL%1,        Young Kyung%Lee%NULL%1,        Hongseok%Ko%NULL%1,        Ki Hwan%Kim%NULL%1,        Chang Min%Park%NULL%1,        Yun-Hyeon%Kim%NULL%1,        Junqiang%Lei%NULL%1,        Jung Hee%Hong%NULL%1,        Hyungjin%Kim%NULL%1,        Eui Jin%Hwang%NULL%1,        Seung Jin%Yoo%NULL%1,        Ju Gang%Nam%NULL%1,        Chang Hyun%Lee%NULL%1,        Jin Mo%Goo%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Yuki%Himoto%yukihimoto@gmail.com%2,         Akihiko%Sakata%NULL%1,         Mitsuhiro%Kirita%NULL%1,         Takashi%Hiroi%NULL%1,         Ken-ichiro%Kobayashi%NULL%1,         Kenji%Kubo%NULL%1,         Hyunjin%Kim%NULL%1,         Azusa%Nishimoto%NULL%1,         Chikara%Maeda%NULL%1,         Akira%Kawamura%NULL%1,         Nobuhiro%Komiya%NULL%1,         Shigeaki%Umeoka%NULL%1,        Yuki%Himoto%yukihimoto@gmail.com%1,        Akihiko%Sakata%NULL%1,        Mitsuhiro%Kirita%NULL%1,        Takashi%Hiroi%NULL%1,        Ken-ichiro%Kobayashi%NULL%1,        Kenji%Kubo%NULL%1,        Hyunjin%Kim%NULL%1,        Azusa%Nishimoto%NULL%1,        Chikara%Maeda%NULL%1,        Akira%Kawamura%NULL%1,        Nobuhiro%Komiya%NULL%1,        Shigeaki%Umeoka%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Chunqin%Long%NULL%2,         Huaxiang%Xu%NULL%1,         Qinglin%Shen%NULL%1,         Xianghai%Zhang%NULL%1,         Bing%Fan%26171381@qq.com%1,         Chuanhong%Wang%NULL%1,         Bingliang%Zeng%NULL%1,         Zicong%Li%NULL%1,         Xiaofen%Li%NULL%1,         Honglu%Li%NULL%1,        Chunqin%Long%NULL%1,        Huaxiang%Xu%NULL%1,        Qinglin%Shen%NULL%1,        Xianghai%Zhang%NULL%1,        Bing%Fan%26171381@qq.com%1,        Chuanhong%Wang%NULL%1,        Bingliang%Zeng%NULL%1,        Zicong%Li%NULL%1,        Xiaofen%Li%NULL%1,        Honglu%Li%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%4,        Christopher%Gieraerts%NULL%1,        Yves%De Bruecker%NULL%1,        Lode%Janssen%NULL%1,        Hanne%Valgaeren%NULL%1,        Dagmar%Obbels%NULL%1,        Marc%Gillis%NULL%1,        Marc%Van Ranst%NULL%0,        Johan%Frans%NULL%1,        Annick%Demeyere%NULL%1,        Rolf%Symons%rolf.symons@imelda.be%1]</t>
-  </si>
-  <si>
-    <t>[Wanbo%Zhu%NULL%0,      Kai%Xie%NULL%0,      Kai%Xie%NULL%0,      Hui%Lu%NULL%0,      Lei%Xu%bayinhexl@126.com%0,      Shusheng%Zhou%zhouss108@163.com%0,      Shiyuan%Fang%fangshiyuan2008@126.com%0]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,      Christopher%Gieraerts%NULL%2,      Christopher%Gieraerts%NULL%0,      Yves%De Bruecker%NULL%2,      Yves%De Bruecker%NULL%0,      Lode%Janssen%NULL%2,      Lode%Janssen%NULL%0,      Hanne%Valgaeren%NULL%2,      Hanne%Valgaeren%NULL%0,      Dagmar%Obbels%NULL%2,      Dagmar%Obbels%NULL%0,      Marc%Gillis%NULL%2,      Marc%Gillis%NULL%0,      Marc%Van Ranst%NULL%0,      Marc%Van Ranst%NULL%0,      Johan%Frans%NULL%1,      Annick%Demeyere%NULL%2,      Annick%Demeyere%NULL%0,      Rolf%Symons%rolf.symons@imelda.be%2,      Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
-    <t>[Harrison X.%Bai%NULL%2,          Ben%Hsieh%NULL%1,          Zeng%Xiong%NULL%1,          Kasey%Halsey%NULL%1,          Ji Whae%Choi%NULL%1,          Thi My Linh%Tran%NULL%1,          Ian%Pan%NULL%1,          Lin-Bo%Shi%NULL%1,          Dong-Cui%Wang%NULL%1,          Ji%Mei%NULL%1,          Xiao-Long%Jiang%NULL%1,          Qiu-Hua%Zeng%NULL%1,          Thomas K.%Egglin%NULL%1,          Ping-Feng%Hu%NULL%1,          Saurabh%Agarwal%NULL%1,          Fangfang%Xie%NULL%1,          Sha%Li%NULL%1,          Terrance%Healey%NULL%1,          Michael K.%Atalay%NULL%1,          Wei-Hua%Liao%liaoweihua2017@163.com%1,         Harrison X.%Bai%NULL%1,         Ben%Hsieh%NULL%1,         Zeng%Xiong%NULL%1,         Kasey%Halsey%NULL%1,         Ji Whae%Choi%NULL%1,         Thi My Linh%Tran%NULL%1,         Ian%Pan%NULL%1,         Lin-Bo%Shi%NULL%1,         Dong-Cui%Wang%NULL%1,         Ji%Mei%NULL%1,         Xiao-Long%Jiang%NULL%1,         Qiu-Hua%Zeng%NULL%1,         Thomas K.%Egglin%NULL%1,         Ping-Feng%Hu%NULL%1,         Saurabh%Agarwal%NULL%1,         Fangfang%Xie%NULL%1,         Sha%Li%NULL%1,         Terrance%Healey%NULL%1,         Michael K.%Atalay%NULL%1,         Wei-Hua%Liao%liaoweihua2017@163.com%1]</t>
-  </si>
-  <si>
-    <t>[Damiano%Caruso%NULL%2,          Marta%Zerunian%NULL%1,          Michela%Polici%NULL%1,          Francesco%Pucciarelli%NULL%1,          Tiziano%Polidori%NULL%1,          Carlotta%Rucci%NULL%1,          Gisella%Guido%NULL%1,          Benedetta%Bracci%NULL%1,          Chiara%de Dominicis%NULL%1,          Andrea%Laghi%andrea.laghi@uniroma1.it%1,         Damiano%Caruso%NULL%1,         Marta%Zerunian%NULL%1,         Michela%Polici%NULL%1,         Francesco%Pucciarelli%NULL%1,         Tiziano%Polidori%NULL%1,         Carlotta%Rucci%NULL%1,         Gisella%Guido%NULL%1,         Benedetta%Bracci%NULL%1,         Chiara%de Dominicis%NULL%1,         Andrea%Laghi%andrea.laghi@uniroma1.it%1]</t>
-  </si>
-  <si>
-    <t>[Xiaofeng%Chen%NULL%2,          Yanyan%Tang%NULL%1,          Yongkang%Mo%NULL%1,          Shengkai%Li%NULL%1,          Daiying%Lin%NULL%1,          Zhijian%Yang%NULL%1,          Zhiqi%Yang%NULL%1,          Hongfu%Sun%NULL%1,          Jinming%Qiu%NULL%1,          Yuting%Liao%NULL%1,          Jianning%Xiao%NULL%1,          Xiangguang%Chen%NULL%1,          Xianheng%Wu%NULL%1,          Renhua%Wu%NULL%1,          Zhuozhi%Dai%zhuozhi@ualberta.ca%1,         Xiaofeng%Chen%NULL%1,         Yanyan%Tang%NULL%1,         Yongkang%Mo%NULL%1,         Shengkai%Li%NULL%1,         Daiying%Lin%NULL%1,         Zhijian%Yang%NULL%1,         Zhiqi%Yang%NULL%1,         Hongfu%Sun%NULL%1,         Jinming%Qiu%NULL%1,         Yuting%Liao%NULL%1,         Jianning%Xiao%NULL%1,         Xiangguang%Chen%NULL%1,         Xianheng%Wu%NULL%1,         Renhua%Wu%NULL%1,         Zhuozhi%Dai%zhuozhi@ualberta.ca%1]</t>
-  </si>
-  <si>
-    <t>[Hyewon%Choi%NULL%2,          Xiaolong%Qi%NULL%1,          Soon Ho%Yoon%yshoka@gmail.com%1,          Sang Joon%Park%NULL%1,          Kyung Hee%Lee%NULL%1,          Jin Yong%Kim%NULL%1,          Young Kyung%Lee%NULL%1,          Hongseok%Ko%NULL%1,          Ki Hwan%Kim%NULL%1,          Chang Min%Park%NULL%1,          Yun-Hyeon%Kim%NULL%1,          Junqiang%Lei%NULL%1,          Jung Hee%Hong%NULL%1,          Hyungjin%Kim%NULL%1,          Eui Jin%Hwang%NULL%1,          Seung Jin%Yoo%NULL%1,          Ju Gang%Nam%NULL%1,          Chang Hyun%Lee%NULL%1,          Jin Mo%Goo%NULL%1,         Hyewon%Choi%NULL%1,         Xiaolong%Qi%NULL%1,         Soon Ho%Yoon%yshoka@gmail.com%1,         Sang Joon%Park%NULL%1,         Kyung Hee%Lee%NULL%1,         Jin Yong%Kim%NULL%1,         Young Kyung%Lee%NULL%1,         Hongseok%Ko%NULL%1,         Ki Hwan%Kim%NULL%1,         Chang Min%Park%NULL%1,         Yun-Hyeon%Kim%NULL%1,         Junqiang%Lei%NULL%1,         Jung Hee%Hong%NULL%1,         Hyungjin%Kim%NULL%1,         Eui Jin%Hwang%NULL%1,         Seung Jin%Yoo%NULL%1,         Ju Gang%Nam%NULL%1,         Chang Hyun%Lee%NULL%1,         Jin Mo%Goo%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Yuki%Himoto%yukihimoto@gmail.com%2,          Akihiko%Sakata%NULL%1,          Mitsuhiro%Kirita%NULL%1,          Takashi%Hiroi%NULL%1,          Ken-ichiro%Kobayashi%NULL%1,          Kenji%Kubo%NULL%1,          Hyunjin%Kim%NULL%1,          Azusa%Nishimoto%NULL%1,          Chikara%Maeda%NULL%1,          Akira%Kawamura%NULL%1,          Nobuhiro%Komiya%NULL%1,          Shigeaki%Umeoka%NULL%1,         Yuki%Himoto%yukihimoto@gmail.com%1,         Akihiko%Sakata%NULL%1,         Mitsuhiro%Kirita%NULL%1,         Takashi%Hiroi%NULL%1,         Ken-ichiro%Kobayashi%NULL%1,         Kenji%Kubo%NULL%1,         Hyunjin%Kim%NULL%1,         Azusa%Nishimoto%NULL%1,         Chikara%Maeda%NULL%1,         Akira%Kawamura%NULL%1,         Nobuhiro%Komiya%NULL%1,         Shigeaki%Umeoka%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Chunqin%Long%NULL%2,          Huaxiang%Xu%NULL%1,          Qinglin%Shen%NULL%1,          Xianghai%Zhang%NULL%1,          Bing%Fan%26171381@qq.com%1,          Chuanhong%Wang%NULL%1,          Bingliang%Zeng%NULL%1,          Zicong%Li%NULL%1,          Xiaofen%Li%NULL%1,          Honglu%Li%NULL%1,         Chunqin%Long%NULL%1,         Huaxiang%Xu%NULL%1,         Qinglin%Shen%NULL%1,         Xianghai%Zhang%NULL%1,         Bing%Fan%26171381@qq.com%1,         Chuanhong%Wang%NULL%1,         Bingliang%Zeng%NULL%1,         Zicong%Li%NULL%1,         Xiaofen%Li%NULL%1,         Honglu%Li%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%4,         Christopher%Gieraerts%NULL%1,         Yves%De Bruecker%NULL%1,         Lode%Janssen%NULL%1,         Hanne%Valgaeren%NULL%1,         Dagmar%Obbels%NULL%1,         Marc%Gillis%NULL%1,         Marc%Van Ranst%NULL%0,         Johan%Frans%NULL%1,         Annick%Demeyere%NULL%1,         Rolf%Symons%rolf.symons@imelda.be%1]</t>
-  </si>
-  <si>
-    <t>[Wanbo%Zhu%NULL%0,       Kai%Xie%NULL%0,       Kai%Xie%NULL%0,       Hui%Lu%NULL%0,       Lei%Xu%bayinhexl@126.com%0,       Shusheng%Zhou%zhouss108@163.com%0,       Shiyuan%Fang%fangshiyuan2008@126.com%0]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,       Christopher%Gieraerts%NULL%2,       Christopher%Gieraerts%NULL%0,       Yves%De Bruecker%NULL%2,       Yves%De Bruecker%NULL%0,       Lode%Janssen%NULL%2,       Lode%Janssen%NULL%0,       Hanne%Valgaeren%NULL%2,       Hanne%Valgaeren%NULL%0,       Dagmar%Obbels%NULL%2,       Dagmar%Obbels%NULL%0,       Marc%Gillis%NULL%2,       Marc%Gillis%NULL%0,       Marc%Van Ranst%NULL%0,       Marc%Van Ranst%NULL%0,       Johan%Frans%NULL%1,       Annick%Demeyere%NULL%2,       Annick%Demeyere%NULL%0,       Rolf%Symons%rolf.symons@imelda.be%2,       Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,    Christopher%Gieraerts%NULL%2,    Christopher%Gieraerts%NULL%0,    Yves%De Bruecker%NULL%2,    Yves%De Bruecker%NULL%0,    Lode%Janssen%NULL%2,    Lode%Janssen%NULL%0,    Hanne%Valgaeren%NULL%2,    Hanne%Valgaeren%NULL%0,    Dagmar%Obbels%NULL%2,    Dagmar%Obbels%NULL%0,    Marc%Gillis%NULL%2,    Marc%Gillis%NULL%0,    Marc%Van Ranst%NULL%2,    Marc%Van Ranst%NULL%0,    Johan%Frans%NULL%1,    Annick%Demeyere%NULL%2,    Annick%Demeyere%NULL%0,    Rolf%Symons%rolf.symons@imelda.be%2,    Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
-    <t>[Harrison X.%Bai%NULL%2,           Ben%Hsieh%NULL%1,           Zeng%Xiong%NULL%1,           Kasey%Halsey%NULL%1,           Ji Whae%Choi%NULL%1,           Thi My Linh%Tran%NULL%1,           Ian%Pan%NULL%1,           Lin-Bo%Shi%NULL%1,           Dong-Cui%Wang%NULL%1,           Ji%Mei%NULL%1,           Xiao-Long%Jiang%NULL%1,           Qiu-Hua%Zeng%NULL%1,           Thomas K.%Egglin%NULL%1,           Ping-Feng%Hu%NULL%1,           Saurabh%Agarwal%NULL%1,           Fangfang%Xie%NULL%1,           Sha%Li%NULL%1,           Terrance%Healey%NULL%1,           Michael K.%Atalay%NULL%1,           Wei-Hua%Liao%liaoweihua2017@163.com%1,          Harrison X.%Bai%NULL%1,          Ben%Hsieh%NULL%1,          Zeng%Xiong%NULL%1,          Kasey%Halsey%NULL%1,          Ji Whae%Choi%NULL%1,          Thi My Linh%Tran%NULL%1,          Ian%Pan%NULL%1,          Lin-Bo%Shi%NULL%1,          Dong-Cui%Wang%NULL%1,          Ji%Mei%NULL%1,          Xiao-Long%Jiang%NULL%1,          Qiu-Hua%Zeng%NULL%1,          Thomas K.%Egglin%NULL%1,          Ping-Feng%Hu%NULL%1,          Saurabh%Agarwal%NULL%1,          Fangfang%Xie%NULL%1,          Sha%Li%NULL%1,          Terrance%Healey%NULL%1,          Michael K.%Atalay%NULL%1,          Wei-Hua%Liao%liaoweihua2017@163.com%1]</t>
-  </si>
-  <si>
-    <t>[Damiano%Caruso%NULL%2,           Marta%Zerunian%NULL%1,           Michela%Polici%NULL%1,           Francesco%Pucciarelli%NULL%1,           Tiziano%Polidori%NULL%1,           Carlotta%Rucci%NULL%1,           Gisella%Guido%NULL%1,           Benedetta%Bracci%NULL%1,           Chiara%de Dominicis%NULL%1,           Andrea%Laghi%andrea.laghi@uniroma1.it%1,          Damiano%Caruso%NULL%1,          Marta%Zerunian%NULL%1,          Michela%Polici%NULL%1,          Francesco%Pucciarelli%NULL%1,          Tiziano%Polidori%NULL%1,          Carlotta%Rucci%NULL%1,          Gisella%Guido%NULL%1,          Benedetta%Bracci%NULL%1,          Chiara%de Dominicis%NULL%1,          Andrea%Laghi%andrea.laghi@uniroma1.it%1]</t>
-  </si>
-  <si>
-    <t>[Xiaofeng%Chen%NULL%2,           Yanyan%Tang%NULL%1,           Yongkang%Mo%NULL%1,           Shengkai%Li%NULL%1,           Daiying%Lin%NULL%1,           Zhijian%Yang%NULL%1,           Zhiqi%Yang%NULL%1,           Hongfu%Sun%NULL%1,           Jinming%Qiu%NULL%1,           Yuting%Liao%NULL%1,           Jianning%Xiao%NULL%1,           Xiangguang%Chen%NULL%1,           Xianheng%Wu%NULL%1,           Renhua%Wu%NULL%1,           Zhuozhi%Dai%zhuozhi@ualberta.ca%1,          Xiaofeng%Chen%NULL%1,          Yanyan%Tang%NULL%1,          Yongkang%Mo%NULL%1,          Shengkai%Li%NULL%1,          Daiying%Lin%NULL%1,          Zhijian%Yang%NULL%1,          Zhiqi%Yang%NULL%1,          Hongfu%Sun%NULL%1,          Jinming%Qiu%NULL%1,          Yuting%Liao%NULL%1,          Jianning%Xiao%NULL%1,          Xiangguang%Chen%NULL%1,          Xianheng%Wu%NULL%1,          Renhua%Wu%NULL%1,          Zhuozhi%Dai%zhuozhi@ualberta.ca%1]</t>
-  </si>
-  <si>
-    <t>[Hyewon%Choi%NULL%2,           Xiaolong%Qi%NULL%1,           Soon Ho%Yoon%yshoka@gmail.com%1,           Sang Joon%Park%NULL%1,           Kyung Hee%Lee%NULL%1,           Jin Yong%Kim%NULL%1,           Young Kyung%Lee%NULL%1,           Hongseok%Ko%NULL%1,           Ki Hwan%Kim%NULL%1,           Chang Min%Park%NULL%1,           Yun-Hyeon%Kim%NULL%1,           Junqiang%Lei%NULL%1,           Jung Hee%Hong%NULL%1,           Hyungjin%Kim%NULL%1,           Eui Jin%Hwang%NULL%1,           Seung Jin%Yoo%NULL%1,           Ju Gang%Nam%NULL%1,           Chang Hyun%Lee%NULL%1,           Jin Mo%Goo%NULL%1,          Hyewon%Choi%NULL%1,          Xiaolong%Qi%NULL%1,          Soon Ho%Yoon%yshoka@gmail.com%1,          Sang Joon%Park%NULL%1,          Kyung Hee%Lee%NULL%1,          Jin Yong%Kim%NULL%1,          Young Kyung%Lee%NULL%1,          Hongseok%Ko%NULL%1,          Ki Hwan%Kim%NULL%1,          Chang Min%Park%NULL%1,          Yun-Hyeon%Kim%NULL%1,          Junqiang%Lei%NULL%1,          Jung Hee%Hong%NULL%1,          Hyungjin%Kim%NULL%1,          Eui Jin%Hwang%NULL%1,          Seung Jin%Yoo%NULL%1,          Ju Gang%Nam%NULL%1,          Chang Hyun%Lee%NULL%1,          Jin Mo%Goo%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Yuki%Himoto%yukihimoto@gmail.com%2,           Akihiko%Sakata%NULL%1,           Mitsuhiro%Kirita%NULL%1,           Takashi%Hiroi%NULL%1,           Ken-ichiro%Kobayashi%NULL%1,           Kenji%Kubo%NULL%1,           Hyunjin%Kim%NULL%1,           Azusa%Nishimoto%NULL%1,           Chikara%Maeda%NULL%1,           Akira%Kawamura%NULL%1,           Nobuhiro%Komiya%NULL%1,           Shigeaki%Umeoka%NULL%1,          Yuki%Himoto%yukihimoto@gmail.com%1,          Akihiko%Sakata%NULL%1,          Mitsuhiro%Kirita%NULL%1,          Takashi%Hiroi%NULL%1,          Ken-ichiro%Kobayashi%NULL%1,          Kenji%Kubo%NULL%1,          Hyunjin%Kim%NULL%1,          Azusa%Nishimoto%NULL%1,          Chikara%Maeda%NULL%1,          Akira%Kawamura%NULL%1,          Nobuhiro%Komiya%NULL%1,          Shigeaki%Umeoka%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Chunqin%Long%NULL%2,           Huaxiang%Xu%NULL%1,           Qinglin%Shen%NULL%1,           Xianghai%Zhang%NULL%1,           Bing%Fan%26171381@qq.com%1,           Chuanhong%Wang%NULL%1,           Bingliang%Zeng%NULL%1,           Zicong%Li%NULL%1,           Xiaofen%Li%NULL%1,           Honglu%Li%NULL%1,          Chunqin%Long%NULL%1,          Huaxiang%Xu%NULL%1,          Qinglin%Shen%NULL%1,          Xianghai%Zhang%NULL%1,          Bing%Fan%26171381@qq.com%1,          Chuanhong%Wang%NULL%1,          Bingliang%Zeng%NULL%1,          Zicong%Li%NULL%1,          Xiaofen%Li%NULL%1,          Honglu%Li%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%4,          Christopher%Gieraerts%NULL%1,          Yves%De Bruecker%NULL%1,          Lode%Janssen%NULL%1,          Hanne%Valgaeren%NULL%1,          Dagmar%Obbels%NULL%1,          Marc%Gillis%NULL%1,          Marc%Van Ranst%NULL%0,          Johan%Frans%NULL%1,          Annick%Demeyere%NULL%1,          Rolf%Symons%rolf.symons@imelda.be%1]</t>
-  </si>
-  <si>
-    <t>[Wanbo%Zhu%NULL%0,        Kai%Xie%NULL%0,        Kai%Xie%NULL%0,        Hui%Lu%NULL%0,        Lei%Xu%bayinhexl@126.com%0,        Shusheng%Zhou%zhouss108@163.com%0,        Shiyuan%Fang%fangshiyuan2008@126.com%0]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,        Christopher%Gieraerts%NULL%2,        Christopher%Gieraerts%NULL%0,        Yves%De Bruecker%NULL%2,        Yves%De Bruecker%NULL%0,        Lode%Janssen%NULL%2,        Lode%Janssen%NULL%0,        Hanne%Valgaeren%NULL%2,        Hanne%Valgaeren%NULL%0,        Dagmar%Obbels%NULL%2,        Dagmar%Obbels%NULL%0,        Marc%Gillis%NULL%2,        Marc%Gillis%NULL%0,        Marc%Van Ranst%NULL%0,        Marc%Van Ranst%NULL%0,        Johan%Frans%NULL%1,        Annick%Demeyere%NULL%2,        Annick%Demeyere%NULL%0,        Rolf%Symons%rolf.symons@imelda.be%2,        Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,     Christopher%Gieraerts%NULL%2,     Christopher%Gieraerts%NULL%0,     Yves%De Bruecker%NULL%2,     Yves%De Bruecker%NULL%0,     Lode%Janssen%NULL%2,     Lode%Janssen%NULL%0,     Hanne%Valgaeren%NULL%2,     Hanne%Valgaeren%NULL%0,     Dagmar%Obbels%NULL%2,     Dagmar%Obbels%NULL%0,     Marc%Gillis%NULL%2,     Marc%Gillis%NULL%0,     Marc%Van Ranst%NULL%2,     Marc%Van Ranst%NULL%0,     Johan%Frans%NULL%1,     Annick%Demeyere%NULL%2,     Annick%Demeyere%NULL%0,     Rolf%Symons%rolf.symons@imelda.be%2,     Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
-    <t>[Harrison X.%Bai%NULL%2,            Ben%Hsieh%NULL%1,            Zeng%Xiong%NULL%1,            Kasey%Halsey%NULL%1,            Ji Whae%Choi%NULL%1,            Thi My Linh%Tran%NULL%1,            Ian%Pan%NULL%1,            Lin-Bo%Shi%NULL%1,            Dong-Cui%Wang%NULL%1,            Ji%Mei%NULL%1,            Xiao-Long%Jiang%NULL%1,            Qiu-Hua%Zeng%NULL%1,            Thomas K.%Egglin%NULL%1,            Ping-Feng%Hu%NULL%1,            Saurabh%Agarwal%NULL%1,            Fangfang%Xie%NULL%1,            Sha%Li%NULL%1,            Terrance%Healey%NULL%1,            Michael K.%Atalay%NULL%1,            Wei-Hua%Liao%liaoweihua2017@163.com%1,           Harrison X.%Bai%NULL%1,           Ben%Hsieh%NULL%1,           Zeng%Xiong%NULL%1,           Kasey%Halsey%NULL%1,           Ji Whae%Choi%NULL%1,           Thi My Linh%Tran%NULL%1,           Ian%Pan%NULL%1,           Lin-Bo%Shi%NULL%1,           Dong-Cui%Wang%NULL%1,           Ji%Mei%NULL%1,           Xiao-Long%Jiang%NULL%1,           Qiu-Hua%Zeng%NULL%1,           Thomas K.%Egglin%NULL%1,           Ping-Feng%Hu%NULL%1,           Saurabh%Agarwal%NULL%1,           Fangfang%Xie%NULL%1,           Sha%Li%NULL%1,           Terrance%Healey%NULL%1,           Michael K.%Atalay%NULL%1,           Wei-Hua%Liao%liaoweihua2017@163.com%1]</t>
-  </si>
-  <si>
-    <t>[Damiano%Caruso%NULL%2,            Marta%Zerunian%NULL%1,            Michela%Polici%NULL%1,            Francesco%Pucciarelli%NULL%1,            Tiziano%Polidori%NULL%1,            Carlotta%Rucci%NULL%1,            Gisella%Guido%NULL%1,            Benedetta%Bracci%NULL%1,            Chiara%de Dominicis%NULL%1,            Andrea%Laghi%andrea.laghi@uniroma1.it%1,           Damiano%Caruso%NULL%1,           Marta%Zerunian%NULL%1,           Michela%Polici%NULL%1,           Francesco%Pucciarelli%NULL%1,           Tiziano%Polidori%NULL%1,           Carlotta%Rucci%NULL%1,           Gisella%Guido%NULL%1,           Benedetta%Bracci%NULL%1,           Chiara%de Dominicis%NULL%1,           Andrea%Laghi%andrea.laghi@uniroma1.it%1]</t>
-  </si>
-  <si>
-    <t>[Xiaofeng%Chen%NULL%2,            Yanyan%Tang%NULL%1,            Yongkang%Mo%NULL%1,            Shengkai%Li%NULL%1,            Daiying%Lin%NULL%1,            Zhijian%Yang%NULL%1,            Zhiqi%Yang%NULL%1,            Hongfu%Sun%NULL%1,            Jinming%Qiu%NULL%1,            Yuting%Liao%NULL%1,            Jianning%Xiao%NULL%1,            Xiangguang%Chen%NULL%1,            Xianheng%Wu%NULL%1,            Renhua%Wu%NULL%1,            Zhuozhi%Dai%zhuozhi@ualberta.ca%1,           Xiaofeng%Chen%NULL%1,           Yanyan%Tang%NULL%1,           Yongkang%Mo%NULL%1,           Shengkai%Li%NULL%1,           Daiying%Lin%NULL%1,           Zhijian%Yang%NULL%1,           Zhiqi%Yang%NULL%1,           Hongfu%Sun%NULL%1,           Jinming%Qiu%NULL%1,           Yuting%Liao%NULL%1,           Jianning%Xiao%NULL%1,           Xiangguang%Chen%NULL%1,           Xianheng%Wu%NULL%1,           Renhua%Wu%NULL%1,           Zhuozhi%Dai%zhuozhi@ualberta.ca%1]</t>
-  </si>
-  <si>
-    <t>[Hyewon%Choi%NULL%2,            Xiaolong%Qi%NULL%1,            Soon Ho%Yoon%yshoka@gmail.com%1,            Sang Joon%Park%NULL%1,            Kyung Hee%Lee%NULL%1,            Jin Yong%Kim%NULL%1,            Young Kyung%Lee%NULL%1,            Hongseok%Ko%NULL%1,            Ki Hwan%Kim%NULL%1,            Chang Min%Park%NULL%1,            Yun-Hyeon%Kim%NULL%1,            Junqiang%Lei%NULL%1,            Jung Hee%Hong%NULL%1,            Hyungjin%Kim%NULL%1,            Eui Jin%Hwang%NULL%1,            Seung Jin%Yoo%NULL%1,            Ju Gang%Nam%NULL%1,            Chang Hyun%Lee%NULL%1,            Jin Mo%Goo%NULL%1,           Hyewon%Choi%NULL%1,           Xiaolong%Qi%NULL%1,           Soon Ho%Yoon%yshoka@gmail.com%1,           Sang Joon%Park%NULL%1,           Kyung Hee%Lee%NULL%1,           Jin Yong%Kim%NULL%1,           Young Kyung%Lee%NULL%1,           Hongseok%Ko%NULL%1,           Ki Hwan%Kim%NULL%1,           Chang Min%Park%NULL%1,           Yun-Hyeon%Kim%NULL%1,           Junqiang%Lei%NULL%1,           Jung Hee%Hong%NULL%1,           Hyungjin%Kim%NULL%1,           Eui Jin%Hwang%NULL%1,           Seung Jin%Yoo%NULL%1,           Ju Gang%Nam%NULL%1,           Chang Hyun%Lee%NULL%1,           Jin Mo%Goo%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Yuki%Himoto%yukihimoto@gmail.com%2,            Akihiko%Sakata%NULL%1,            Mitsuhiro%Kirita%NULL%1,            Takashi%Hiroi%NULL%1,            Ken-ichiro%Kobayashi%NULL%1,            Kenji%Kubo%NULL%1,            Hyunjin%Kim%NULL%1,            Azusa%Nishimoto%NULL%1,            Chikara%Maeda%NULL%1,            Akira%Kawamura%NULL%1,            Nobuhiro%Komiya%NULL%1,            Shigeaki%Umeoka%NULL%1,           Yuki%Himoto%yukihimoto@gmail.com%1,           Akihiko%Sakata%NULL%1,           Mitsuhiro%Kirita%NULL%1,           Takashi%Hiroi%NULL%1,           Ken-ichiro%Kobayashi%NULL%1,           Kenji%Kubo%NULL%1,           Hyunjin%Kim%NULL%1,           Azusa%Nishimoto%NULL%1,           Chikara%Maeda%NULL%1,           Akira%Kawamura%NULL%1,           Nobuhiro%Komiya%NULL%1,           Shigeaki%Umeoka%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Chunqin%Long%NULL%2,            Huaxiang%Xu%NULL%1,            Qinglin%Shen%NULL%1,            Xianghai%Zhang%NULL%1,            Bing%Fan%26171381@qq.com%1,            Chuanhong%Wang%NULL%1,            Bingliang%Zeng%NULL%1,            Zicong%Li%NULL%1,            Xiaofen%Li%NULL%1,            Honglu%Li%NULL%1,           Chunqin%Long%NULL%1,           Huaxiang%Xu%NULL%1,           Qinglin%Shen%NULL%1,           Xianghai%Zhang%NULL%1,           Bing%Fan%26171381@qq.com%1,           Chuanhong%Wang%NULL%1,           Bingliang%Zeng%NULL%1,           Zicong%Li%NULL%1,           Xiaofen%Li%NULL%1,           Honglu%Li%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%4,           Christopher%Gieraerts%NULL%1,           Yves%De Bruecker%NULL%1,           Lode%Janssen%NULL%1,           Hanne%Valgaeren%NULL%1,           Dagmar%Obbels%NULL%1,           Marc%Gillis%NULL%1,           Marc%Van Ranst%NULL%0,           Johan%Frans%NULL%1,           Annick%Demeyere%NULL%1,           Rolf%Symons%rolf.symons@imelda.be%1]</t>
-  </si>
-  <si>
-    <t>[Wanbo%Zhu%NULL%0,         Kai%Xie%NULL%0,         Kai%Xie%NULL%0,         Hui%Lu%NULL%0,         Lei%Xu%bayinhexl@126.com%0,         Shusheng%Zhou%zhouss108@163.com%0,         Shiyuan%Fang%fangshiyuan2008@126.com%0]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,         Christopher%Gieraerts%NULL%2,         Christopher%Gieraerts%NULL%0,         Yves%De Bruecker%NULL%2,         Yves%De Bruecker%NULL%0,         Lode%Janssen%NULL%2,         Lode%Janssen%NULL%0,         Hanne%Valgaeren%NULL%2,         Hanne%Valgaeren%NULL%0,         Dagmar%Obbels%NULL%2,         Dagmar%Obbels%NULL%0,         Marc%Gillis%NULL%2,         Marc%Gillis%NULL%0,         Marc%Van Ranst%NULL%0,         Marc%Van Ranst%NULL%0,         Johan%Frans%NULL%1,         Annick%Demeyere%NULL%2,         Annick%Demeyere%NULL%0,         Rolf%Symons%rolf.symons@imelda.be%2,         Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,      Christopher%Gieraerts%NULL%2,      Christopher%Gieraerts%NULL%0,      Yves%De Bruecker%NULL%2,      Yves%De Bruecker%NULL%0,      Lode%Janssen%NULL%2,      Lode%Janssen%NULL%0,      Hanne%Valgaeren%NULL%2,      Hanne%Valgaeren%NULL%0,      Dagmar%Obbels%NULL%2,      Dagmar%Obbels%NULL%0,      Marc%Gillis%NULL%2,      Marc%Gillis%NULL%0,      Marc%Van Ranst%NULL%2,      Marc%Van Ranst%NULL%0,      Johan%Frans%NULL%1,      Annick%Demeyere%NULL%2,      Annick%Demeyere%NULL%0,      Rolf%Symons%rolf.symons@imelda.be%2,      Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
-    <t>[Harrison X.%Bai%NULL%2,             Ben%Hsieh%NULL%1,             Zeng%Xiong%NULL%1,             Kasey%Halsey%NULL%1,             Ji Whae%Choi%NULL%1,             Thi My Linh%Tran%NULL%1,             Ian%Pan%NULL%1,             Lin-Bo%Shi%NULL%1,             Dong-Cui%Wang%NULL%1,             Ji%Mei%NULL%1,             Xiao-Long%Jiang%NULL%1,             Qiu-Hua%Zeng%NULL%1,             Thomas K.%Egglin%NULL%1,             Ping-Feng%Hu%NULL%1,             Saurabh%Agarwal%NULL%1,             Fangfang%Xie%NULL%1,             Sha%Li%NULL%1,             Terrance%Healey%NULL%1,             Michael K.%Atalay%NULL%1,             Wei-Hua%Liao%liaoweihua2017@163.com%1,            Harrison X.%Bai%NULL%1,            Ben%Hsieh%NULL%1,            Zeng%Xiong%NULL%1,            Kasey%Halsey%NULL%1,            Ji Whae%Choi%NULL%1,            Thi My Linh%Tran%NULL%1,            Ian%Pan%NULL%1,            Lin-Bo%Shi%NULL%1,            Dong-Cui%Wang%NULL%1,            Ji%Mei%NULL%1,            Xiao-Long%Jiang%NULL%1,            Qiu-Hua%Zeng%NULL%1,            Thomas K.%Egglin%NULL%1,            Ping-Feng%Hu%NULL%1,            Saurabh%Agarwal%NULL%1,            Fangfang%Xie%NULL%1,            Sha%Li%NULL%1,            Terrance%Healey%NULL%1,            Michael K.%Atalay%NULL%1,            Wei-Hua%Liao%liaoweihua2017@163.com%1]</t>
-  </si>
-  <si>
-    <t>[Damiano%Caruso%NULL%2,             Marta%Zerunian%NULL%1,             Michela%Polici%NULL%1,             Francesco%Pucciarelli%NULL%1,             Tiziano%Polidori%NULL%1,             Carlotta%Rucci%NULL%1,             Gisella%Guido%NULL%1,             Benedetta%Bracci%NULL%1,             Chiara%de Dominicis%NULL%1,             Andrea%Laghi%andrea.laghi@uniroma1.it%1,            Damiano%Caruso%NULL%1,            Marta%Zerunian%NULL%1,            Michela%Polici%NULL%1,            Francesco%Pucciarelli%NULL%1,            Tiziano%Polidori%NULL%1,            Carlotta%Rucci%NULL%1,            Gisella%Guido%NULL%1,            Benedetta%Bracci%NULL%1,            Chiara%de Dominicis%NULL%1,            Andrea%Laghi%andrea.laghi@uniroma1.it%1]</t>
-  </si>
-  <si>
-    <t>[Xiaofeng%Chen%NULL%2,             Yanyan%Tang%NULL%1,             Yongkang%Mo%NULL%1,             Shengkai%Li%NULL%1,             Daiying%Lin%NULL%1,             Zhijian%Yang%NULL%1,             Zhiqi%Yang%NULL%1,             Hongfu%Sun%NULL%1,             Jinming%Qiu%NULL%1,             Yuting%Liao%NULL%1,             Jianning%Xiao%NULL%1,             Xiangguang%Chen%NULL%1,             Xianheng%Wu%NULL%1,             Renhua%Wu%NULL%1,             Zhuozhi%Dai%zhuozhi@ualberta.ca%1,            Xiaofeng%Chen%NULL%1,            Yanyan%Tang%NULL%1,            Yongkang%Mo%NULL%1,            Shengkai%Li%NULL%1,            Daiying%Lin%NULL%1,            Zhijian%Yang%NULL%1,            Zhiqi%Yang%NULL%1,            Hongfu%Sun%NULL%1,            Jinming%Qiu%NULL%1,            Yuting%Liao%NULL%1,            Jianning%Xiao%NULL%1,            Xiangguang%Chen%NULL%1,            Xianheng%Wu%NULL%1,            Renhua%Wu%NULL%1,            Zhuozhi%Dai%zhuozhi@ualberta.ca%1]</t>
-  </si>
-  <si>
-    <t>[Hyewon%Choi%NULL%2,             Xiaolong%Qi%NULL%1,             Soon Ho%Yoon%yshoka@gmail.com%1,             Sang Joon%Park%NULL%1,             Kyung Hee%Lee%NULL%1,             Jin Yong%Kim%NULL%1,             Young Kyung%Lee%NULL%1,             Hongseok%Ko%NULL%1,             Ki Hwan%Kim%NULL%1,             Chang Min%Park%NULL%1,             Yun-Hyeon%Kim%NULL%1,             Junqiang%Lei%NULL%1,             Jung Hee%Hong%NULL%1,             Hyungjin%Kim%NULL%1,             Eui Jin%Hwang%NULL%1,             Seung Jin%Yoo%NULL%1,             Ju Gang%Nam%NULL%1,             Chang Hyun%Lee%NULL%1,             Jin Mo%Goo%NULL%1,            Hyewon%Choi%NULL%1,            Xiaolong%Qi%NULL%1,            Soon Ho%Yoon%yshoka@gmail.com%1,            Sang Joon%Park%NULL%1,            Kyung Hee%Lee%NULL%1,            Jin Yong%Kim%NULL%1,            Young Kyung%Lee%NULL%1,            Hongseok%Ko%NULL%1,            Ki Hwan%Kim%NULL%1,            Chang Min%Park%NULL%1,            Yun-Hyeon%Kim%NULL%1,            Junqiang%Lei%NULL%1,            Jung Hee%Hong%NULL%1,            Hyungjin%Kim%NULL%1,            Eui Jin%Hwang%NULL%1,            Seung Jin%Yoo%NULL%1,            Ju Gang%Nam%NULL%1,            Chang Hyun%Lee%NULL%1,            Jin Mo%Goo%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Yuki%Himoto%yukihimoto@gmail.com%2,             Akihiko%Sakata%NULL%1,             Mitsuhiro%Kirita%NULL%1,             Takashi%Hiroi%NULL%1,             Ken-ichiro%Kobayashi%NULL%1,             Kenji%Kubo%NULL%1,             Hyunjin%Kim%NULL%1,             Azusa%Nishimoto%NULL%1,             Chikara%Maeda%NULL%1,             Akira%Kawamura%NULL%1,             Nobuhiro%Komiya%NULL%1,             Shigeaki%Umeoka%NULL%1,            Yuki%Himoto%yukihimoto@gmail.com%1,            Akihiko%Sakata%NULL%1,            Mitsuhiro%Kirita%NULL%1,            Takashi%Hiroi%NULL%1,            Ken-ichiro%Kobayashi%NULL%1,            Kenji%Kubo%NULL%1,            Hyunjin%Kim%NULL%1,            Azusa%Nishimoto%NULL%1,            Chikara%Maeda%NULL%1,            Akira%Kawamura%NULL%1,            Nobuhiro%Komiya%NULL%1,            Shigeaki%Umeoka%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Chunqin%Long%NULL%2,             Huaxiang%Xu%NULL%1,             Qinglin%Shen%NULL%1,             Xianghai%Zhang%NULL%1,             Bing%Fan%26171381@qq.com%1,             Chuanhong%Wang%NULL%1,             Bingliang%Zeng%NULL%1,             Zicong%Li%NULL%1,             Xiaofen%Li%NULL%1,             Honglu%Li%NULL%1,            Chunqin%Long%NULL%1,            Huaxiang%Xu%NULL%1,            Qinglin%Shen%NULL%1,            Xianghai%Zhang%NULL%1,            Bing%Fan%26171381@qq.com%1,            Chuanhong%Wang%NULL%1,            Bingliang%Zeng%NULL%1,            Zicong%Li%NULL%1,            Xiaofen%Li%NULL%1,            Honglu%Li%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%4,            Christopher%Gieraerts%NULL%1,            Yves%De Bruecker%NULL%1,            Lode%Janssen%NULL%1,            Hanne%Valgaeren%NULL%1,            Dagmar%Obbels%NULL%1,            Marc%Gillis%NULL%1,            Marc%Van Ranst%NULL%0,            Johan%Frans%NULL%1,            Annick%Demeyere%NULL%1,            Rolf%Symons%rolf.symons@imelda.be%1]</t>
-  </si>
-  <si>
-    <t>[Wanbo%Zhu%NULL%0,          Kai%Xie%NULL%0,          Kai%Xie%NULL%0,          Hui%Lu%NULL%0,          Lei%Xu%bayinhexl@126.com%0,          Shusheng%Zhou%zhouss108@163.com%0,          Shiyuan%Fang%fangshiyuan2008@126.com%0]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,          Christopher%Gieraerts%NULL%2,          Christopher%Gieraerts%NULL%0,          Yves%De Bruecker%NULL%2,          Yves%De Bruecker%NULL%0,          Lode%Janssen%NULL%2,          Lode%Janssen%NULL%0,          Hanne%Valgaeren%NULL%2,          Hanne%Valgaeren%NULL%0,          Dagmar%Obbels%NULL%2,          Dagmar%Obbels%NULL%0,          Marc%Gillis%NULL%2,          Marc%Gillis%NULL%0,          Marc%Van Ranst%NULL%0,          Marc%Van Ranst%NULL%0,          Johan%Frans%NULL%1,          Annick%Demeyere%NULL%2,          Annick%Demeyere%NULL%0,          Rolf%Symons%rolf.symons@imelda.be%2,          Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,       Christopher%Gieraerts%NULL%2,       Christopher%Gieraerts%NULL%0,       Yves%De Bruecker%NULL%2,       Yves%De Bruecker%NULL%0,       Lode%Janssen%NULL%2,       Lode%Janssen%NULL%0,       Hanne%Valgaeren%NULL%2,       Hanne%Valgaeren%NULL%0,       Dagmar%Obbels%NULL%2,       Dagmar%Obbels%NULL%0,       Marc%Gillis%NULL%2,       Marc%Gillis%NULL%0,       Marc%Van Ranst%NULL%2,       Marc%Van Ranst%NULL%0,       Johan%Frans%NULL%1,       Annick%Demeyere%NULL%2,       Annick%Demeyere%NULL%0,       Rolf%Symons%rolf.symons@imelda.be%2,       Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
-    <t>[Harrison X.%Bai%NULL%2,              Ben%Hsieh%NULL%1,              Zeng%Xiong%NULL%1,              Kasey%Halsey%NULL%1,              Ji Whae%Choi%NULL%1,              Thi My Linh%Tran%NULL%1,              Ian%Pan%NULL%1,              Lin-Bo%Shi%NULL%1,              Dong-Cui%Wang%NULL%1,              Ji%Mei%NULL%1,              Xiao-Long%Jiang%NULL%1,              Qiu-Hua%Zeng%NULL%1,              Thomas K.%Egglin%NULL%1,              Ping-Feng%Hu%NULL%1,              Saurabh%Agarwal%NULL%1,              Fangfang%Xie%NULL%1,              Sha%Li%NULL%1,              Terrance%Healey%NULL%1,              Michael K.%Atalay%NULL%1,              Wei-Hua%Liao%liaoweihua2017@163.com%1,             Harrison X.%Bai%NULL%1,             Ben%Hsieh%NULL%1,             Zeng%Xiong%NULL%1,             Kasey%Halsey%NULL%1,             Ji Whae%Choi%NULL%1,             Thi My Linh%Tran%NULL%1,             Ian%Pan%NULL%1,             Lin-Bo%Shi%NULL%1,             Dong-Cui%Wang%NULL%1,             Ji%Mei%NULL%1,             Xiao-Long%Jiang%NULL%1,             Qiu-Hua%Zeng%NULL%1,             Thomas K.%Egglin%NULL%1,             Ping-Feng%Hu%NULL%1,             Saurabh%Agarwal%NULL%1,             Fangfang%Xie%NULL%1,             Sha%Li%NULL%1,             Terrance%Healey%NULL%1,             Michael K.%Atalay%NULL%1,             Wei-Hua%Liao%liaoweihua2017@163.com%1]</t>
-  </si>
-  <si>
-    <t>[Damiano%Caruso%NULL%2,              Marta%Zerunian%NULL%1,              Michela%Polici%NULL%1,              Francesco%Pucciarelli%NULL%1,              Tiziano%Polidori%NULL%1,              Carlotta%Rucci%NULL%1,              Gisella%Guido%NULL%1,              Benedetta%Bracci%NULL%1,              Chiara%de Dominicis%NULL%1,              Andrea%Laghi%andrea.laghi@uniroma1.it%1,             Damiano%Caruso%NULL%1,             Marta%Zerunian%NULL%1,             Michela%Polici%NULL%1,             Francesco%Pucciarelli%NULL%1,             Tiziano%Polidori%NULL%1,             Carlotta%Rucci%NULL%1,             Gisella%Guido%NULL%1,             Benedetta%Bracci%NULL%1,             Chiara%de Dominicis%NULL%1,             Andrea%Laghi%andrea.laghi@uniroma1.it%1]</t>
-  </si>
-  <si>
-    <t>[Xiaofeng%Chen%NULL%2,              Yanyan%Tang%NULL%1,              Yongkang%Mo%NULL%1,              Shengkai%Li%NULL%1,              Daiying%Lin%NULL%1,              Zhijian%Yang%NULL%1,              Zhiqi%Yang%NULL%1,              Hongfu%Sun%NULL%1,              Jinming%Qiu%NULL%1,              Yuting%Liao%NULL%1,              Jianning%Xiao%NULL%1,              Xiangguang%Chen%NULL%1,              Xianheng%Wu%NULL%1,              Renhua%Wu%NULL%1,              Zhuozhi%Dai%zhuozhi@ualberta.ca%1,             Xiaofeng%Chen%NULL%1,             Yanyan%Tang%NULL%1,             Yongkang%Mo%NULL%1,             Shengkai%Li%NULL%1,             Daiying%Lin%NULL%1,             Zhijian%Yang%NULL%1,             Zhiqi%Yang%NULL%1,             Hongfu%Sun%NULL%1,             Jinming%Qiu%NULL%1,             Yuting%Liao%NULL%1,             Jianning%Xiao%NULL%1,             Xiangguang%Chen%NULL%1,             Xianheng%Wu%NULL%1,             Renhua%Wu%NULL%1,             Zhuozhi%Dai%zhuozhi@ualberta.ca%1]</t>
-  </si>
-  <si>
-    <t>[Hyewon%Choi%NULL%2,              Xiaolong%Qi%NULL%1,              Soon Ho%Yoon%yshoka@gmail.com%1,              Sang Joon%Park%NULL%1,              Kyung Hee%Lee%NULL%1,              Jin Yong%Kim%NULL%1,              Young Kyung%Lee%NULL%1,              Hongseok%Ko%NULL%1,              Ki Hwan%Kim%NULL%1,              Chang Min%Park%NULL%1,              Yun-Hyeon%Kim%NULL%1,              Junqiang%Lei%NULL%1,              Jung Hee%Hong%NULL%1,              Hyungjin%Kim%NULL%1,              Eui Jin%Hwang%NULL%1,              Seung Jin%Yoo%NULL%1,              Ju Gang%Nam%NULL%1,              Chang Hyun%Lee%NULL%1,              Jin Mo%Goo%NULL%1,             Hyewon%Choi%NULL%1,             Xiaolong%Qi%NULL%1,             Soon Ho%Yoon%yshoka@gmail.com%1,             Sang Joon%Park%NULL%1,             Kyung Hee%Lee%NULL%1,             Jin Yong%Kim%NULL%1,             Young Kyung%Lee%NULL%1,             Hongseok%Ko%NULL%1,             Ki Hwan%Kim%NULL%1,             Chang Min%Park%NULL%1,             Yun-Hyeon%Kim%NULL%1,             Junqiang%Lei%NULL%1,             Jung Hee%Hong%NULL%1,             Hyungjin%Kim%NULL%1,             Eui Jin%Hwang%NULL%1,             Seung Jin%Yoo%NULL%1,             Ju Gang%Nam%NULL%1,             Chang Hyun%Lee%NULL%1,             Jin Mo%Goo%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Yuki%Himoto%yukihimoto@gmail.com%2,              Akihiko%Sakata%NULL%1,              Mitsuhiro%Kirita%NULL%1,              Takashi%Hiroi%NULL%1,              Ken-ichiro%Kobayashi%NULL%1,              Kenji%Kubo%NULL%1,              Hyunjin%Kim%NULL%1,              Azusa%Nishimoto%NULL%1,              Chikara%Maeda%NULL%1,              Akira%Kawamura%NULL%1,              Nobuhiro%Komiya%NULL%1,              Shigeaki%Umeoka%NULL%1,             Yuki%Himoto%yukihimoto@gmail.com%1,             Akihiko%Sakata%NULL%1,             Mitsuhiro%Kirita%NULL%1,             Takashi%Hiroi%NULL%1,             Ken-ichiro%Kobayashi%NULL%1,             Kenji%Kubo%NULL%1,             Hyunjin%Kim%NULL%1,             Azusa%Nishimoto%NULL%1,             Chikara%Maeda%NULL%1,             Akira%Kawamura%NULL%1,             Nobuhiro%Komiya%NULL%1,             Shigeaki%Umeoka%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Chunqin%Long%NULL%2,              Huaxiang%Xu%NULL%1,              Qinglin%Shen%NULL%1,              Xianghai%Zhang%NULL%1,              Bing%Fan%26171381@qq.com%1,              Chuanhong%Wang%NULL%1,              Bingliang%Zeng%NULL%1,              Zicong%Li%NULL%1,              Xiaofen%Li%NULL%1,              Honglu%Li%NULL%1,             Chunqin%Long%NULL%1,             Huaxiang%Xu%NULL%1,             Qinglin%Shen%NULL%1,             Xianghai%Zhang%NULL%1,             Bing%Fan%26171381@qq.com%1,             Chuanhong%Wang%NULL%1,             Bingliang%Zeng%NULL%1,             Zicong%Li%NULL%1,             Xiaofen%Li%NULL%1,             Honglu%Li%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%4,             Christopher%Gieraerts%NULL%1,             Yves%De Bruecker%NULL%1,             Lode%Janssen%NULL%1,             Hanne%Valgaeren%NULL%1,             Dagmar%Obbels%NULL%1,             Marc%Gillis%NULL%1,             Marc%Van Ranst%NULL%0,             Johan%Frans%NULL%1,             Annick%Demeyere%NULL%1,             Rolf%Symons%rolf.symons@imelda.be%1]</t>
-  </si>
-  <si>
-    <t>[Wanbo%Zhu%NULL%0,           Kai%Xie%NULL%0,           Kai%Xie%NULL%0,           Hui%Lu%NULL%0,           Lei%Xu%bayinhexl@126.com%0,           Shusheng%Zhou%zhouss108@163.com%0,           Shiyuan%Fang%fangshiyuan2008@126.com%0]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,           Christopher%Gieraerts%NULL%2,           Christopher%Gieraerts%NULL%0,           Yves%De Bruecker%NULL%2,           Yves%De Bruecker%NULL%0,           Lode%Janssen%NULL%2,           Lode%Janssen%NULL%0,           Hanne%Valgaeren%NULL%2,           Hanne%Valgaeren%NULL%0,           Dagmar%Obbels%NULL%2,           Dagmar%Obbels%NULL%0,           Marc%Gillis%NULL%2,           Marc%Gillis%NULL%0,           Marc%Van Ranst%NULL%0,           Marc%Van Ranst%NULL%0,           Johan%Frans%NULL%1,           Annick%Demeyere%NULL%2,           Annick%Demeyere%NULL%0,           Rolf%Symons%rolf.symons@imelda.be%2,           Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,        Christopher%Gieraerts%NULL%2,        Christopher%Gieraerts%NULL%0,        Yves%De Bruecker%NULL%2,        Yves%De Bruecker%NULL%0,        Lode%Janssen%NULL%2,        Lode%Janssen%NULL%0,        Hanne%Valgaeren%NULL%2,        Hanne%Valgaeren%NULL%0,        Dagmar%Obbels%NULL%2,        Dagmar%Obbels%NULL%0,        Marc%Gillis%NULL%2,        Marc%Gillis%NULL%0,        Marc%Van Ranst%NULL%2,        Marc%Van Ranst%NULL%0,        Johan%Frans%NULL%1,        Annick%Demeyere%NULL%2,        Annick%Demeyere%NULL%0,        Rolf%Symons%rolf.symons@imelda.be%2,        Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
-    <t>[Harrison X.%Bai%NULL%2,               Ben%Hsieh%NULL%1,               Zeng%Xiong%NULL%1,               Kasey%Halsey%NULL%1,               Ji Whae%Choi%NULL%1,               Thi My Linh%Tran%NULL%1,               Ian%Pan%NULL%1,               Lin-Bo%Shi%NULL%1,               Dong-Cui%Wang%NULL%1,               Ji%Mei%NULL%1,               Xiao-Long%Jiang%NULL%1,               Qiu-Hua%Zeng%NULL%1,               Thomas K.%Egglin%NULL%1,               Ping-Feng%Hu%NULL%1,               Saurabh%Agarwal%NULL%1,               Fangfang%Xie%NULL%1,               Sha%Li%NULL%1,               Terrance%Healey%NULL%1,               Michael K.%Atalay%NULL%1,               Wei-Hua%Liao%liaoweihua2017@163.com%1,              Harrison X.%Bai%NULL%1,              Ben%Hsieh%NULL%1,              Zeng%Xiong%NULL%1,              Kasey%Halsey%NULL%1,              Ji Whae%Choi%NULL%1,              Thi My Linh%Tran%NULL%1,              Ian%Pan%NULL%1,              Lin-Bo%Shi%NULL%1,              Dong-Cui%Wang%NULL%1,              Ji%Mei%NULL%1,              Xiao-Long%Jiang%NULL%1,              Qiu-Hua%Zeng%NULL%1,              Thomas K.%Egglin%NULL%1,              Ping-Feng%Hu%NULL%1,              Saurabh%Agarwal%NULL%1,              Fangfang%Xie%NULL%1,              Sha%Li%NULL%1,              Terrance%Healey%NULL%1,              Michael K.%Atalay%NULL%1,              Wei-Hua%Liao%liaoweihua2017@163.com%1]</t>
-  </si>
-  <si>
-    <t>[Damiano%Caruso%NULL%2,               Marta%Zerunian%NULL%1,               Michela%Polici%NULL%1,               Francesco%Pucciarelli%NULL%1,               Tiziano%Polidori%NULL%1,               Carlotta%Rucci%NULL%1,               Gisella%Guido%NULL%1,               Benedetta%Bracci%NULL%1,               Chiara%de Dominicis%NULL%1,               Andrea%Laghi%andrea.laghi@uniroma1.it%1,              Damiano%Caruso%NULL%1,              Marta%Zerunian%NULL%1,              Michela%Polici%NULL%1,              Francesco%Pucciarelli%NULL%1,              Tiziano%Polidori%NULL%1,              Carlotta%Rucci%NULL%1,              Gisella%Guido%NULL%1,              Benedetta%Bracci%NULL%1,              Chiara%de Dominicis%NULL%1,              Andrea%Laghi%andrea.laghi@uniroma1.it%1]</t>
-  </si>
-  <si>
-    <t>[Xiaofeng%Chen%NULL%2,               Yanyan%Tang%NULL%1,               Yongkang%Mo%NULL%1,               Shengkai%Li%NULL%1,               Daiying%Lin%NULL%1,               Zhijian%Yang%NULL%1,               Zhiqi%Yang%NULL%1,               Hongfu%Sun%NULL%1,               Jinming%Qiu%NULL%1,               Yuting%Liao%NULL%1,               Jianning%Xiao%NULL%1,               Xiangguang%Chen%NULL%1,               Xianheng%Wu%NULL%1,               Renhua%Wu%NULL%1,               Zhuozhi%Dai%zhuozhi@ualberta.ca%1,              Xiaofeng%Chen%NULL%1,              Yanyan%Tang%NULL%1,              Yongkang%Mo%NULL%1,              Shengkai%Li%NULL%1,              Daiying%Lin%NULL%1,              Zhijian%Yang%NULL%1,              Zhiqi%Yang%NULL%1,              Hongfu%Sun%NULL%1,              Jinming%Qiu%NULL%1,              Yuting%Liao%NULL%1,              Jianning%Xiao%NULL%1,              Xiangguang%Chen%NULL%1,              Xianheng%Wu%NULL%1,              Renhua%Wu%NULL%1,              Zhuozhi%Dai%zhuozhi@ualberta.ca%1]</t>
-  </si>
-  <si>
-    <t>[Hyewon%Choi%NULL%2,               Xiaolong%Qi%NULL%1,               Soon Ho%Yoon%yshoka@gmail.com%1,               Sang Joon%Park%NULL%1,               Kyung Hee%Lee%NULL%1,               Jin Yong%Kim%NULL%1,               Young Kyung%Lee%NULL%1,               Hongseok%Ko%NULL%1,               Ki Hwan%Kim%NULL%1,               Chang Min%Park%NULL%1,               Yun-Hyeon%Kim%NULL%1,               Junqiang%Lei%NULL%1,               Jung Hee%Hong%NULL%1,               Hyungjin%Kim%NULL%1,               Eui Jin%Hwang%NULL%1,               Seung Jin%Yoo%NULL%1,               Ju Gang%Nam%NULL%1,               Chang Hyun%Lee%NULL%1,               Jin Mo%Goo%NULL%1,              Hyewon%Choi%NULL%1,              Xiaolong%Qi%NULL%1,              Soon Ho%Yoon%yshoka@gmail.com%1,              Sang Joon%Park%NULL%1,              Kyung Hee%Lee%NULL%1,              Jin Yong%Kim%NULL%1,              Young Kyung%Lee%NULL%1,              Hongseok%Ko%NULL%1,              Ki Hwan%Kim%NULL%1,              Chang Min%Park%NULL%1,              Yun-Hyeon%Kim%NULL%1,              Junqiang%Lei%NULL%1,              Jung Hee%Hong%NULL%1,              Hyungjin%Kim%NULL%1,              Eui Jin%Hwang%NULL%1,              Seung Jin%Yoo%NULL%1,              Ju Gang%Nam%NULL%1,              Chang Hyun%Lee%NULL%1,              Jin Mo%Goo%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Yuki%Himoto%yukihimoto@gmail.com%2,               Akihiko%Sakata%NULL%1,               Mitsuhiro%Kirita%NULL%1,               Takashi%Hiroi%NULL%1,               Ken-ichiro%Kobayashi%NULL%1,               Kenji%Kubo%NULL%1,               Hyunjin%Kim%NULL%1,               Azusa%Nishimoto%NULL%1,               Chikara%Maeda%NULL%1,               Akira%Kawamura%NULL%1,               Nobuhiro%Komiya%NULL%1,               Shigeaki%Umeoka%NULL%1,              Yuki%Himoto%yukihimoto@gmail.com%1,              Akihiko%Sakata%NULL%1,              Mitsuhiro%Kirita%NULL%1,              Takashi%Hiroi%NULL%1,              Ken-ichiro%Kobayashi%NULL%1,              Kenji%Kubo%NULL%1,              Hyunjin%Kim%NULL%1,              Azusa%Nishimoto%NULL%1,              Chikara%Maeda%NULL%1,              Akira%Kawamura%NULL%1,              Nobuhiro%Komiya%NULL%1,              Shigeaki%Umeoka%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Chunqin%Long%NULL%2,               Huaxiang%Xu%NULL%1,               Qinglin%Shen%NULL%1,               Xianghai%Zhang%NULL%1,               Bing%Fan%26171381@qq.com%1,               Chuanhong%Wang%NULL%1,               Bingliang%Zeng%NULL%1,               Zicong%Li%NULL%1,               Xiaofen%Li%NULL%1,               Honglu%Li%NULL%1,              Chunqin%Long%NULL%1,              Huaxiang%Xu%NULL%1,              Qinglin%Shen%NULL%1,              Xianghai%Zhang%NULL%1,              Bing%Fan%26171381@qq.com%1,              Chuanhong%Wang%NULL%1,              Bingliang%Zeng%NULL%1,              Zicong%Li%NULL%1,              Xiaofen%Li%NULL%1,              Honglu%Li%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%4,              Christopher%Gieraerts%NULL%1,              Yves%De Bruecker%NULL%1,              Lode%Janssen%NULL%1,              Hanne%Valgaeren%NULL%1,              Dagmar%Obbels%NULL%1,              Marc%Gillis%NULL%1,              Marc%Van Ranst%NULL%0,              Johan%Frans%NULL%1,              Annick%Demeyere%NULL%1,              Rolf%Symons%rolf.symons@imelda.be%1]</t>
-  </si>
-  <si>
-    <t>[Wanbo%Zhu%NULL%0,            Kai%Xie%NULL%0,            Kai%Xie%NULL%0,            Hui%Lu%NULL%0,            Lei%Xu%bayinhexl@126.com%0,            Shusheng%Zhou%zhouss108@163.com%0,            Shiyuan%Fang%fangshiyuan2008@126.com%0]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,            Christopher%Gieraerts%NULL%2,            Christopher%Gieraerts%NULL%0,            Yves%De Bruecker%NULL%2,            Yves%De Bruecker%NULL%0,            Lode%Janssen%NULL%2,            Lode%Janssen%NULL%0,            Hanne%Valgaeren%NULL%2,            Hanne%Valgaeren%NULL%0,            Dagmar%Obbels%NULL%2,            Dagmar%Obbels%NULL%0,            Marc%Gillis%NULL%2,            Marc%Gillis%NULL%0,            Marc%Van Ranst%NULL%0,            Marc%Van Ranst%NULL%0,            Johan%Frans%NULL%1,            Annick%Demeyere%NULL%2,            Annick%Demeyere%NULL%0,            Rolf%Symons%rolf.symons@imelda.be%2,            Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,         Christopher%Gieraerts%NULL%2,         Christopher%Gieraerts%NULL%0,         Yves%De Bruecker%NULL%2,         Yves%De Bruecker%NULL%0,         Lode%Janssen%NULL%2,         Lode%Janssen%NULL%0,         Hanne%Valgaeren%NULL%2,         Hanne%Valgaeren%NULL%0,         Dagmar%Obbels%NULL%2,         Dagmar%Obbels%NULL%0,         Marc%Gillis%NULL%2,         Marc%Gillis%NULL%0,         Marc%Van Ranst%NULL%2,         Marc%Van Ranst%NULL%0,         Johan%Frans%NULL%1,         Annick%Demeyere%NULL%2,         Annick%Demeyere%NULL%0,         Rolf%Symons%rolf.symons@imelda.be%2,         Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
-    <t>[Harrison X.%Bai%NULL%2,                Ben%Hsieh%NULL%1,                Zeng%Xiong%NULL%1,                Kasey%Halsey%NULL%1,                Ji Whae%Choi%NULL%1,                Thi My Linh%Tran%NULL%1,                Ian%Pan%NULL%1,                Lin-Bo%Shi%NULL%1,                Dong-Cui%Wang%NULL%1,                Ji%Mei%NULL%1,                Xiao-Long%Jiang%NULL%1,                Qiu-Hua%Zeng%NULL%1,                Thomas K.%Egglin%NULL%1,                Ping-Feng%Hu%NULL%1,                Saurabh%Agarwal%NULL%1,                Fangfang%Xie%NULL%1,                Sha%Li%NULL%1,                Terrance%Healey%NULL%1,                Michael K.%Atalay%NULL%1,                Wei-Hua%Liao%liaoweihua2017@163.com%1,               Harrison X.%Bai%NULL%1,               Ben%Hsieh%NULL%1,               Zeng%Xiong%NULL%1,               Kasey%Halsey%NULL%1,               Ji Whae%Choi%NULL%1,               Thi My Linh%Tran%NULL%1,               Ian%Pan%NULL%1,               Lin-Bo%Shi%NULL%1,               Dong-Cui%Wang%NULL%1,               Ji%Mei%NULL%1,               Xiao-Long%Jiang%NULL%1,               Qiu-Hua%Zeng%NULL%1,               Thomas K.%Egglin%NULL%1,               Ping-Feng%Hu%NULL%1,               Saurabh%Agarwal%NULL%1,               Fangfang%Xie%NULL%1,               Sha%Li%NULL%1,               Terrance%Healey%NULL%1,               Michael K.%Atalay%NULL%1,               Wei-Hua%Liao%liaoweihua2017@163.com%1]</t>
-  </si>
-  <si>
-    <t>[Damiano%Caruso%NULL%2,                Marta%Zerunian%NULL%1,                Michela%Polici%NULL%1,                Francesco%Pucciarelli%NULL%1,                Tiziano%Polidori%NULL%1,                Carlotta%Rucci%NULL%1,                Gisella%Guido%NULL%1,                Benedetta%Bracci%NULL%1,                Chiara%de Dominicis%NULL%1,                Andrea%Laghi%andrea.laghi@uniroma1.it%1,               Damiano%Caruso%NULL%1,               Marta%Zerunian%NULL%1,               Michela%Polici%NULL%1,               Francesco%Pucciarelli%NULL%1,               Tiziano%Polidori%NULL%1,               Carlotta%Rucci%NULL%1,               Gisella%Guido%NULL%1,               Benedetta%Bracci%NULL%1,               Chiara%de Dominicis%NULL%1,               Andrea%Laghi%andrea.laghi@uniroma1.it%1]</t>
   </si>
   <si>
     <t xml:space="preserve">Objectives
@@ -730,12 +331,6 @@
 </t>
   </si>
   <si>
-    <t>[Xiaofeng%Chen%NULL%2,                Yanyan%Tang%NULL%1,                Yongkang%Mo%NULL%1,                Shengkai%Li%NULL%1,                Daiying%Lin%NULL%1,                Zhijian%Yang%NULL%1,                Zhiqi%Yang%NULL%1,                Hongfu%Sun%NULL%1,                Jinming%Qiu%NULL%1,                Yuting%Liao%NULL%1,                Jianning%Xiao%NULL%1,                Xiangguang%Chen%NULL%1,                Xianheng%Wu%NULL%1,                Renhua%Wu%NULL%1,                Zhuozhi%Dai%zhuozhi@ualberta.ca%1,               Xiaofeng%Chen%NULL%1,               Yanyan%Tang%NULL%1,               Yongkang%Mo%NULL%1,               Shengkai%Li%NULL%1,               Daiying%Lin%NULL%1,               Zhijian%Yang%NULL%1,               Zhiqi%Yang%NULL%1,               Hongfu%Sun%NULL%1,               Jinming%Qiu%NULL%1,               Yuting%Liao%NULL%1,               Jianning%Xiao%NULL%1,               Xiangguang%Chen%NULL%1,               Xianheng%Wu%NULL%1,               Renhua%Wu%NULL%1,               Zhuozhi%Dai%zhuozhi@ualberta.ca%1]</t>
-  </si>
-  <si>
-    <t>[Hyewon%Choi%NULL%2,                Xiaolong%Qi%NULL%1,                Soon Ho%Yoon%yshoka@gmail.com%1,                Sang Joon%Park%NULL%1,                Kyung Hee%Lee%NULL%1,                Jin Yong%Kim%NULL%1,                Young Kyung%Lee%NULL%1,                Hongseok%Ko%NULL%1,                Ki Hwan%Kim%NULL%1,                Chang Min%Park%NULL%1,                Yun-Hyeon%Kim%NULL%1,                Junqiang%Lei%NULL%1,                Jung Hee%Hong%NULL%1,                Hyungjin%Kim%NULL%1,                Eui Jin%Hwang%NULL%1,                Seung Jin%Yoo%NULL%1,                Ju Gang%Nam%NULL%1,                Chang Hyun%Lee%NULL%1,                Jin Mo%Goo%NULL%1,               Hyewon%Choi%NULL%1,               Xiaolong%Qi%NULL%1,               Soon Ho%Yoon%yshoka@gmail.com%1,               Sang Joon%Park%NULL%1,               Kyung Hee%Lee%NULL%1,               Jin Yong%Kim%NULL%1,               Young Kyung%Lee%NULL%1,               Hongseok%Ko%NULL%1,               Ki Hwan%Kim%NULL%1,               Chang Min%Park%NULL%1,               Yun-Hyeon%Kim%NULL%1,               Junqiang%Lei%NULL%1,               Jung Hee%Hong%NULL%1,               Hyungjin%Kim%NULL%1,               Eui Jin%Hwang%NULL%1,               Seung Jin%Yoo%NULL%1,               Ju Gang%Nam%NULL%1,               Chang Hyun%Lee%NULL%1,               Jin Mo%Goo%NULL%1]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Purpose
 To evaluate the diagnostic performance of chest CT to differentiate coronavirus disease 2019 (COVID-19) pneumonia in non-high-epidemic area in Japan.
 Materials and methods
@@ -751,24 +346,6 @@
 </t>
   </si>
   <si>
-    <t>[Yuki%Himoto%yukihimoto@gmail.com%2,                Akihiko%Sakata%NULL%1,                Mitsuhiro%Kirita%NULL%1,                Takashi%Hiroi%NULL%1,                Ken-ichiro%Kobayashi%NULL%1,                Kenji%Kubo%NULL%1,                Hyunjin%Kim%NULL%1,                Azusa%Nishimoto%NULL%1,                Chikara%Maeda%NULL%1,                Akira%Kawamura%NULL%1,                Nobuhiro%Komiya%NULL%1,                Shigeaki%Umeoka%NULL%1,               Yuki%Himoto%yukihimoto@gmail.com%1,               Akihiko%Sakata%NULL%1,               Mitsuhiro%Kirita%NULL%1,               Takashi%Hiroi%NULL%1,               Ken-ichiro%Kobayashi%NULL%1,               Kenji%Kubo%NULL%1,               Hyunjin%Kim%NULL%1,               Azusa%Nishimoto%NULL%1,               Chikara%Maeda%NULL%1,               Akira%Kawamura%NULL%1,               Nobuhiro%Komiya%NULL%1,               Shigeaki%Umeoka%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Chunqin%Long%NULL%2,                Huaxiang%Xu%NULL%1,                Qinglin%Shen%NULL%1,                Xianghai%Zhang%NULL%1,                Bing%Fan%26171381@qq.com%1,                Chuanhong%Wang%NULL%1,                Bingliang%Zeng%NULL%1,                Zicong%Li%NULL%1,                Xiaofen%Li%NULL%1,                Honglu%Li%NULL%1,               Chunqin%Long%NULL%1,               Huaxiang%Xu%NULL%1,               Qinglin%Shen%NULL%1,               Xianghai%Zhang%NULL%1,               Bing%Fan%26171381@qq.com%1,               Chuanhong%Wang%NULL%1,               Bingliang%Zeng%NULL%1,               Zicong%Li%NULL%1,               Xiaofen%Li%NULL%1,               Honglu%Li%NULL%1]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%4,               Christopher%Gieraerts%NULL%1,               Yves%De Bruecker%NULL%1,               Lode%Janssen%NULL%1,               Hanne%Valgaeren%NULL%1,               Dagmar%Obbels%NULL%1,               Marc%Gillis%NULL%1,               Marc%Van Ranst%NULL%0,               Johan%Frans%NULL%1,               Annick%Demeyere%NULL%1,               Rolf%Symons%rolf.symons@imelda.be%1]</t>
-  </si>
-  <si>
-    <t>[Wanbo%Zhu%NULL%0,             Kai%Xie%NULL%0,             Kai%Xie%NULL%0,             Hui%Lu%NULL%0,             Lei%Xu%bayinhexl@126.com%0,             Shusheng%Zhou%zhouss108@163.com%0,             Shiyuan%Fang%fangshiyuan2008@126.com%0]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,             Christopher%Gieraerts%NULL%2,             Christopher%Gieraerts%NULL%0,             Yves%De Bruecker%NULL%2,             Yves%De Bruecker%NULL%0,             Lode%Janssen%NULL%2,             Lode%Janssen%NULL%0,             Hanne%Valgaeren%NULL%2,             Hanne%Valgaeren%NULL%0,             Dagmar%Obbels%NULL%2,             Dagmar%Obbels%NULL%0,             Marc%Gillis%NULL%2,             Marc%Gillis%NULL%0,             Marc%Van Ranst%NULL%0,             Marc%Van Ranst%NULL%0,             Johan%Frans%NULL%1,             Annick%Demeyere%NULL%2,             Annick%Demeyere%NULL%0,             Rolf%Symons%rolf.symons@imelda.be%2,             Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
-    <t>[Anthony%Dangis%NULL%0,          Christopher%Gieraerts%NULL%2,          Christopher%Gieraerts%NULL%0,          Yves%De Bruecker%NULL%2,          Yves%De Bruecker%NULL%0,          Lode%Janssen%NULL%2,          Lode%Janssen%NULL%0,          Hanne%Valgaeren%NULL%2,          Hanne%Valgaeren%NULL%0,          Dagmar%Obbels%NULL%2,          Dagmar%Obbels%NULL%0,          Marc%Gillis%NULL%2,          Marc%Gillis%NULL%0,          Marc%Van Ranst%NULL%2,          Marc%Van Ranst%NULL%0,          Johan%Frans%NULL%1,          Annick%Demeyere%NULL%2,          Annick%Demeyere%NULL%0,          Rolf%Symons%rolf.symons@imelda.be%2,          Rolf%Symons%rolf.symons@imelda.be%0]</t>
-  </si>
-  <si>
     <t>[Harrison X.%Bai%NULL%2,                 Ben%Hsieh%NULL%1,                 Zeng%Xiong%NULL%1,                 Kasey%Halsey%NULL%1,                 Ji Whae%Choi%NULL%1,                 Thi My Linh%Tran%NULL%1,                 Ian%Pan%NULL%1,                 Lin-Bo%Shi%NULL%1,                 Dong-Cui%Wang%NULL%1,                 Ji%Mei%NULL%1,                 Xiao-Long%Jiang%NULL%1,                 Qiu-Hua%Zeng%NULL%1,                 Thomas K.%Egglin%NULL%1,                 Ping-Feng%Hu%NULL%1,                 Saurabh%Agarwal%NULL%1,                 Fangfang%Xie%NULL%1,                 Sha%Li%NULL%1,                 Terrance%Healey%NULL%1,                 Michael K.%Atalay%NULL%1,                 Wei-Hua%Liao%liaoweihua2017@163.com%1,                Harrison X.%Bai%NULL%1,                Ben%Hsieh%NULL%1,                Zeng%Xiong%NULL%1,                Kasey%Halsey%NULL%1,                Ji Whae%Choi%NULL%1,                Thi My Linh%Tran%NULL%1,                Ian%Pan%NULL%1,                Lin-Bo%Shi%NULL%1,                Dong-Cui%Wang%NULL%1,                Ji%Mei%NULL%1,                Xiao-Long%Jiang%NULL%1,                Qiu-Hua%Zeng%NULL%1,                Thomas K.%Egglin%NULL%1,                Ping-Feng%Hu%NULL%1,                Saurabh%Agarwal%NULL%1,                Fangfang%Xie%NULL%1,                Sha%Li%NULL%1,                Terrance%Healey%NULL%1,                Michael K.%Atalay%NULL%1,                Wei-Hua%Liao%liaoweihua2017@163.com%1]</t>
   </si>
   <si>
@@ -797,6 +374,12 @@
   </si>
   <si>
     <t>[Anthony%Dangis%NULL%0,           Christopher%Gieraerts%NULL%2,           Christopher%Gieraerts%NULL%0,           Yves%De Bruecker%NULL%2,           Yves%De Bruecker%NULL%0,           Lode%Janssen%NULL%2,           Lode%Janssen%NULL%0,           Hanne%Valgaeren%NULL%2,           Hanne%Valgaeren%NULL%0,           Dagmar%Obbels%NULL%2,           Dagmar%Obbels%NULL%0,           Marc%Gillis%NULL%2,           Marc%Gillis%NULL%0,           Marc%Van Ranst%NULL%2,           Marc%Van Ranst%NULL%0,           Johan%Frans%NULL%1,           Annick%Demeyere%NULL%2,           Annick%Demeyere%NULL%0,           Rolf%Symons%rolf.symons@imelda.be%2,           Rolf%Symons%rolf.symons@imelda.be%0]</t>
+  </si>
+  <si>
+    <t>10.1148/radiol.2020200642</t>
+  </si>
+  <si>
+    <t>10.2214/AJR.20.22959</t>
   </si>
 </sst>
 </file>
@@ -1066,15 +649,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1082,28 +665,28 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1111,344 +694,344 @@
         <v>44044</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>191</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="B3" s="2">
         <v>44044</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" t="s">
-        <v>32</v>
-      </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
         <v>44044</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>192</v>
+        <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3">
         <v>43937</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>181</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>193</v>
+        <v>64</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="B6" s="2">
         <v>44013</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
         <v>30</v>
       </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>32</v>
-      </c>
       <c r="H6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>43922</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>194</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4">
         <v>43952</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>184</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>195</v>
+        <v>66</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="4">
         <v>43952</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>196</v>
+        <v>67</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B10" s="2">
         <v>44348</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
-        <v>197</v>
+        <v>68</v>
       </c>
       <c r="F10" t="s">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2">
         <v>43922</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" t="s">
         <v>54</v>
       </c>
-      <c r="E11" t="s">
-        <v>198</v>
-      </c>
-      <c r="F11" t="s">
-        <v>98</v>
-      </c>
-      <c r="G11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2">
         <v>44075</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>199</v>
+        <v>70</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2">
         <v>43922</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" t="s">
         <v>55</v>
-      </c>
-      <c r="E13" t="s">
-        <v>200</v>
-      </c>
-      <c r="F13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" t="s">
-        <v>47</v>
-      </c>
-      <c r="I13" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>